<commit_message>
Convert code from notebook to python source + new classifiers
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Projects/Seal-Pup-Aerial-Imagery-Classifier/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A28D6E9F-B9A2-E54E-96F3-459B84D5E46E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD03910E-E900-A747-8517-9ED01D330567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{077603D1-627F-BB4C-8452-0B21DBAC2288}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="8">
   <si>
     <t>Average accuracy</t>
   </si>
@@ -51,6 +51,12 @@
   </si>
   <si>
     <t>HoG + RGB</t>
+  </si>
+  <si>
+    <t>Linear SVC</t>
+  </si>
+  <si>
+    <t>SGD</t>
   </si>
 </sst>
 </file>
@@ -403,55 +409,78 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB18750C-C232-5147-A52A-F477DF1E1291}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1">
+      <c r="C2" s="1">
         <v>0.88090000000000002</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="1">
+      <c r="C3" s="1">
         <v>0.96130000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="1">
+      <c r="C4" s="1">
         <v>0.80659999999999998</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="1">
+      <c r="C5" s="1">
         <v>0.86370000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="1">
+        <v>0.81669999999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add pyspinners + minor improvements
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Projects/Seal-Pup-Aerial-Imagery-Classifier/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD03910E-E900-A747-8517-9ED01D330567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0763613-C0B9-9745-AF04-727001990384}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{077603D1-627F-BB4C-8452-0B21DBAC2288}"/>
   </bookViews>
@@ -412,7 +412,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Grid search code + results on multi-MLP
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Projects/Seal-Pup-Aerial-Imagery-Classifier/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{554A2B08-72CC-2C4A-BA06-49C03997A7AB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AFE66F8-1610-5C43-B63D-A9EBD65251FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19320" xr2:uid="{077603D1-627F-BB4C-8452-0B21DBAC2288}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19280" activeTab="7" xr2:uid="{077603D1-627F-BB4C-8452-0B21DBAC2288}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,8 +20,12 @@
     <sheet name="Poly SVC" sheetId="5" r:id="rId5"/>
     <sheet name="Decision Tree" sheetId="7" r:id="rId6"/>
     <sheet name="MLP" sheetId="6" r:id="rId7"/>
+    <sheet name="MLP Multi GS" sheetId="8" r:id="rId8"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MLP Multi GS'!$A$1:$S$1</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="300" uniqueCount="114">
   <si>
     <t>Average accuracy</t>
   </si>
@@ -86,15 +90,18 @@
     <t>Multi</t>
   </si>
   <si>
-    <t>Polynomial SVC</t>
+    <t>Decision Tree</t>
+  </si>
+  <si>
+    <t>Neural Network</t>
+  </si>
+  <si>
+    <t>(using 3-fold cross validation)</t>
   </si>
   <si>
     <t>Runtime (s)</t>
   </si>
   <si>
-    <t>(using 3-fold cross validation, all processors)</t>
-  </si>
-  <si>
     <t>Convergence warnings</t>
   </si>
   <si>
@@ -107,35 +114,284 @@
     <t>Max # iterations</t>
   </si>
   <si>
-    <t>*not using all processors</t>
-  </si>
-  <si>
-    <t>Linear SVC*</t>
-  </si>
-  <si>
-    <t>Logistic (OvR)</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
     <t>Too long</t>
   </si>
   <si>
-    <t>Neural Network*</t>
-  </si>
-  <si>
     <t>∞</t>
   </si>
   <si>
-    <t>Decision Tree*</t>
+    <t>SGD*</t>
+  </si>
+  <si>
+    <t>Logistic (OvR)*</t>
+  </si>
+  <si>
+    <t>Polynomial SVC*</t>
+  </si>
+  <si>
+    <t>*using all processors</t>
+  </si>
+  <si>
+    <t>Best model hyperparameters found by randomised search algorithm:</t>
+  </si>
+  <si>
+    <t>MLPClassifier(activation='relu', alpha=0.0001, batch_size='auto', beta_1=0.9,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              beta_2=0.999, early_stopping=False, epsilon=1e-08,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              hidden_layer_sizes=(1000,), learning_rate='constant',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              learning_rate_init=0.1, max_fun=15000, max_iter=200, momentum=0.1,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              n_iter_no_change=10, nesterovs_momentum=True, power_t=0.5,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              random_state=111, shuffle=True, solver='adam', tol=0.0001,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              validation_fraction=0.1, verbose=False, warm_start=False)</t>
+  </si>
+  <si>
+    <t>--- Training Runtime: 30145.05 seconds ---</t>
+  </si>
+  <si>
+    <t>mean_fit_time</t>
+  </si>
+  <si>
+    <t>std_fit_time</t>
+  </si>
+  <si>
+    <t>mean_score_time</t>
+  </si>
+  <si>
+    <t>std_score_time</t>
+  </si>
+  <si>
+    <t>param_activation</t>
+  </si>
+  <si>
+    <t>param_hidden_layer_sizes</t>
+  </si>
+  <si>
+    <t>param_learning_rate_init</t>
+  </si>
+  <si>
+    <t>param_momentum</t>
+  </si>
+  <si>
+    <t>params</t>
+  </si>
+  <si>
+    <t>split0_test_score</t>
+  </si>
+  <si>
+    <t>split1_test_score</t>
+  </si>
+  <si>
+    <t>split2_test_score</t>
+  </si>
+  <si>
+    <t>mean_test_score</t>
+  </si>
+  <si>
+    <t>std_test_score</t>
+  </si>
+  <si>
+    <t>rank_test_score</t>
+  </si>
+  <si>
+    <t>relu</t>
+  </si>
+  <si>
+    <t>(100,)</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.1, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.1, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.1, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.5, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.5, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.5, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 1.0, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 1.0, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (100,), 'learning_rate_init': 1.0, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>(475,)</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.1, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.1, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.1, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.5, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.5, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.5, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 1.0, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 1.0, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (475,), 'learning_rate_init': 1.0, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>(1000,)</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.1, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.1, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.1, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.5, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.5, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.5, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 1.0, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 1.0, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'relu', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 1.0, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>tanh</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.1, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.1, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.1, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.5, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.5, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 0.5, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 1.0, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 1.0, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (100,), 'learning_rate_init': 1.0, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.1, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.1, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.1, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.5, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.5, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 0.5, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 1.0, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 1.0, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (475,), 'learning_rate_init': 1.0, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.1, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.1, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.1, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.5, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.5, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 0.5, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 1.0, 'momentum': 0.1}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 1.0, 'momentum': 0.5}</t>
+  </si>
+  <si>
+    <t>{'activation': 'tanh', 'hidden_layer_sizes': (1000,), 'learning_rate_init': 1.0, 'momentum': 1.0}</t>
+  </si>
+  <si>
+    <t>hours</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,6 +411,25 @@
       <color theme="1"/>
       <name val="Cambria Math"/>
       <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -177,16 +452,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -208,7 +487,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>882650</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>107950</xdr:rowOff>
@@ -220,6 +499,61 @@
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
               <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{BF3080C1-2DCD-1F40-BEE0-379A6D5A0687}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="10064750" y="4781550"/>
+          <a:ext cx="65" cy="172227"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>882650</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>107950</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="65" cy="172227"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="40" name="TextBox 39">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3EE5A544-CC54-5F40-A0C3-9F97E835E092}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2043,17 +2377,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB18750C-C232-5147-A52A-F477DF1E1291}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F34" sqref="F34"/>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.5" customWidth="1"/>
     <col min="2" max="3" width="15.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.33203125" customWidth="1"/>
+    <col min="6" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2129,30 +2464,30 @@
       <c r="A10" t="s">
         <v>1</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3" t="s">
+      <c r="B10" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C10" s="7"/>
+      <c r="D10" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="E10" s="7"/>
+      <c r="F10" s="7" t="s">
+        <v>6</v>
+      </c>
+      <c r="G10" s="7"/>
+      <c r="H10" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="7"/>
+      <c r="J10" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="M10" s="3"/>
+      <c r="K10" s="7"/>
+      <c r="L10" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="M10" s="7"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
@@ -2221,7 +2556,7 @@
         <v>0.31580000000000003</v>
       </c>
       <c r="I12" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J12" s="1">
         <v>0.92579999999999996</v>
@@ -2262,7 +2597,7 @@
         <v>0.14960000000000001</v>
       </c>
       <c r="I13" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J13" s="1">
         <v>0.70630000000000004</v>
@@ -2303,7 +2638,7 @@
         <v>0.95459999999999989</v>
       </c>
       <c r="I14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J14" s="1">
         <v>0.69589999999999996</v>
@@ -2344,7 +2679,7 @@
         <v>0.25869999999999999</v>
       </c>
       <c r="I15" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="J15" s="1">
         <v>0.70109999999999995</v>
@@ -2361,140 +2696,538 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B16" s="4">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3">
         <v>70.28</v>
       </c>
-      <c r="C16" s="4">
+      <c r="C16" s="3">
         <v>294.35000000000002</v>
       </c>
-      <c r="D16" s="4">
+      <c r="D16" s="3">
         <v>104.41</v>
       </c>
-      <c r="E16" s="4">
+      <c r="E16" s="3">
         <v>136.55000000000001</v>
       </c>
-      <c r="F16" s="4">
+      <c r="F16" s="3">
         <v>160.09</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>656.8</v>
       </c>
-      <c r="H16" s="4">
+      <c r="H16" s="3">
         <v>252.95</v>
       </c>
       <c r="I16" t="s">
-        <v>25</v>
-      </c>
-      <c r="J16" s="4">
+        <v>23</v>
+      </c>
+      <c r="J16" s="3">
         <v>442.02</v>
       </c>
-      <c r="K16" s="4">
+      <c r="K16" s="3">
         <v>540.11</v>
       </c>
-      <c r="L16" s="4">
+      <c r="L16" s="3">
         <v>13.58</v>
       </c>
-      <c r="M16" s="4">
+      <c r="M16" s="3">
         <v>187.61</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>21</v>
-      </c>
-      <c r="B17" s="5">
+        <v>22</v>
+      </c>
+      <c r="B17" s="4">
         <v>10000</v>
       </c>
-      <c r="C17" s="5">
+      <c r="C17" s="4">
         <v>10000</v>
       </c>
-      <c r="D17" s="5">
+      <c r="D17" s="4">
         <v>100</v>
       </c>
-      <c r="E17" s="5">
+      <c r="E17" s="4">
         <v>100</v>
       </c>
-      <c r="F17" s="5">
+      <c r="F17" s="4">
         <v>1000</v>
       </c>
-      <c r="G17" s="5">
+      <c r="G17" s="4">
         <v>1000</v>
       </c>
-      <c r="H17" s="5">
+      <c r="H17" s="4">
         <v>1000</v>
       </c>
-      <c r="I17" s="5">
+      <c r="I17" s="4">
         <v>10000</v>
       </c>
-      <c r="J17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="K17" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="L17" s="4">
+      <c r="J17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K17" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="L17" s="3">
         <v>100</v>
       </c>
-      <c r="M17" s="4">
+      <c r="M17" s="3">
         <v>100</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B18" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C18" t="s">
+        <v>21</v>
+      </c>
+      <c r="D18" t="s">
+        <v>21</v>
+      </c>
+      <c r="E18" t="s">
+        <v>21</v>
+      </c>
+      <c r="F18" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" t="s">
+        <v>21</v>
+      </c>
+      <c r="H18" t="s">
+        <v>21</v>
+      </c>
+      <c r="I18" t="s">
+        <v>24</v>
+      </c>
+      <c r="J18" t="s">
         <v>20</v>
       </c>
-      <c r="D18" t="s">
+      <c r="K18" t="s">
         <v>20</v>
       </c>
-      <c r="E18" t="s">
+      <c r="L18" t="s">
         <v>20</v>
       </c>
-      <c r="F18" t="s">
-        <v>20</v>
-      </c>
-      <c r="G18" t="s">
-        <v>20</v>
-      </c>
-      <c r="H18" t="s">
-        <v>20</v>
-      </c>
-      <c r="I18" t="s">
-        <v>26</v>
-      </c>
-      <c r="J18" t="s">
-        <v>19</v>
-      </c>
-      <c r="K18" t="s">
-        <v>19</v>
-      </c>
-      <c r="L18" t="s">
-        <v>19</v>
-      </c>
       <c r="M18" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A22" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
+        <v>1</v>
+      </c>
+      <c r="B24" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D24" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" s="1">
+        <v>0.95879999999999999</v>
+      </c>
+      <c r="C25" s="1">
+        <v>0.96619999999999995</v>
+      </c>
+      <c r="D25" s="1">
+        <v>0.95889999999999997</v>
+      </c>
+      <c r="E25" s="1">
+        <v>0.31580000000000003</v>
+      </c>
+      <c r="F25" s="1">
+        <v>0.92579999999999996</v>
+      </c>
+      <c r="G25" s="1">
+        <v>0.93589999999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A26" t="s">
+        <v>9</v>
+      </c>
+      <c r="B26" s="1">
+        <v>0.87419999999999998</v>
+      </c>
+      <c r="C26" s="1">
+        <v>0.91139999999999999</v>
+      </c>
+      <c r="D26" s="1">
+        <v>0.87219999999999998</v>
+      </c>
+      <c r="E26" s="1">
+        <v>0.14960000000000001</v>
+      </c>
+      <c r="F26" s="1">
+        <v>0.70630000000000004</v>
+      </c>
+      <c r="G26" s="1">
+        <v>0.75980000000000003</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" s="1">
+        <v>0.78269999999999995</v>
+      </c>
+      <c r="C27" s="1">
+        <v>0.80859999999999999</v>
+      </c>
+      <c r="D27" s="1">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="E27" s="1">
+        <v>0.95459999999999989</v>
+      </c>
+      <c r="F27" s="1">
+        <v>0.69589999999999996</v>
+      </c>
+      <c r="G27" s="1">
+        <v>0.71279999999999999</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A28" t="s">
+        <v>11</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.82589999999999997</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.8569</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.82740000000000002</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.25869999999999999</v>
+      </c>
+      <c r="F28" s="1">
+        <v>0.70109999999999995</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.73550000000000004</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A29" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="3">
+        <v>70.28</v>
+      </c>
+      <c r="C29" s="3">
+        <v>104.41</v>
+      </c>
+      <c r="D29" s="3">
+        <v>160.09</v>
+      </c>
+      <c r="E29" s="3">
+        <v>252.95</v>
+      </c>
+      <c r="F29" s="3">
+        <v>442.02</v>
+      </c>
+      <c r="G29" s="3">
+        <v>13.58</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A30" t="s">
         <v>22</v>
+      </c>
+      <c r="B30" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C30" s="4">
+        <v>100</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1000</v>
+      </c>
+      <c r="F30" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G30" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A31" t="s">
+        <v>19</v>
+      </c>
+      <c r="B31" t="s">
+        <v>20</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>21</v>
+      </c>
+      <c r="E31" t="s">
+        <v>21</v>
+      </c>
+      <c r="F31" t="s">
+        <v>20</v>
+      </c>
+      <c r="G31" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>1</v>
+      </c>
+      <c r="B36" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C36" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E36" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" s="1">
+        <v>0.93020000000000003</v>
+      </c>
+      <c r="C37" s="1">
+        <v>0.9395</v>
+      </c>
+      <c r="D37" s="1">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="E37" t="s">
+        <v>23</v>
+      </c>
+      <c r="F37" s="1">
+        <v>0.88490000000000002</v>
+      </c>
+      <c r="G37" s="1">
+        <v>0.91849999999999998</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>9</v>
+      </c>
+      <c r="B38" s="1">
+        <v>0.91410000000000002</v>
+      </c>
+      <c r="C38" s="1">
+        <v>0.93259999999999998</v>
+      </c>
+      <c r="D38" s="1">
+        <v>0.92420000000000002</v>
+      </c>
+      <c r="E38" t="s">
+        <v>23</v>
+      </c>
+      <c r="F38" s="1">
+        <v>0.88790000000000002</v>
+      </c>
+      <c r="G38" s="1">
+        <v>0.90629999999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>10</v>
+      </c>
+      <c r="B39" s="1">
+        <v>0.93020000000000003</v>
+      </c>
+      <c r="C39" s="1">
+        <v>0.9395</v>
+      </c>
+      <c r="D39" s="1">
+        <v>0.93669999999999998</v>
+      </c>
+      <c r="E39" t="s">
+        <v>23</v>
+      </c>
+      <c r="F39" s="1">
+        <v>0.88490000000000002</v>
+      </c>
+      <c r="G39" s="1">
+        <v>0.91859999999999997</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>11</v>
+      </c>
+      <c r="B40" s="1">
+        <v>0.91690000000000005</v>
+      </c>
+      <c r="C40" s="1">
+        <v>0.93500000000000005</v>
+      </c>
+      <c r="D40" s="1">
+        <v>0.92709999999999992</v>
+      </c>
+      <c r="E40" t="s">
+        <v>23</v>
+      </c>
+      <c r="F40" s="1">
+        <v>0.88639999999999997</v>
+      </c>
+      <c r="G40" s="1">
+        <v>0.90800000000000003</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>18</v>
+      </c>
+      <c r="B41" s="3">
+        <v>294.35000000000002</v>
+      </c>
+      <c r="C41" s="3">
+        <v>136.55000000000001</v>
+      </c>
+      <c r="D41" s="3">
+        <v>656.8</v>
+      </c>
+      <c r="E41" t="s">
+        <v>23</v>
+      </c>
+      <c r="F41" s="3">
+        <v>540.11</v>
+      </c>
+      <c r="G41" s="3">
+        <v>187.61</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>22</v>
+      </c>
+      <c r="B42" s="4">
+        <v>10000</v>
+      </c>
+      <c r="C42" s="4">
+        <v>100</v>
+      </c>
+      <c r="D42" s="4">
+        <v>1000</v>
+      </c>
+      <c r="E42" s="4">
+        <v>10000</v>
+      </c>
+      <c r="F42" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="G42" s="3">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>19</v>
+      </c>
+      <c r="B43" t="s">
+        <v>21</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>21</v>
+      </c>
+      <c r="E43" t="s">
+        <v>24</v>
+      </c>
+      <c r="F43" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
+    <mergeCell ref="L10:M10"/>
     <mergeCell ref="B10:C10"/>
     <mergeCell ref="D10:E10"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:I10"/>
     <mergeCell ref="J10:K10"/>
-    <mergeCell ref="L10:M10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -2589,4 +3322,2821 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D934D3DC-A5C6-4745-8A18-4A11C09A9C22}">
+  <dimension ref="A1:S55"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8" customWidth="1"/>
+    <col min="11" max="14" width="15" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.1640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A1" s="8"/>
+      <c r="B1" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J1" s="9" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="9" t="s">
+        <v>48</v>
+      </c>
+      <c r="L1" s="9" t="s">
+        <v>49</v>
+      </c>
+      <c r="M1" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="N1" s="9" t="s">
+        <v>51</v>
+      </c>
+      <c r="O1" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="P1" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="R1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
+        <v>18</v>
+      </c>
+      <c r="B2" s="10">
+        <v>535.45661950111401</v>
+      </c>
+      <c r="C2" s="10">
+        <v>0.39484010467519798</v>
+      </c>
+      <c r="D2" s="10">
+        <v>0.36647017796834302</v>
+      </c>
+      <c r="E2" s="10">
+        <v>6.50972079666643E-3</v>
+      </c>
+      <c r="F2" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G2" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H2" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I2" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>76</v>
+      </c>
+      <c r="K2" s="10">
+        <v>0.94126699713732398</v>
+      </c>
+      <c r="L2" s="10">
+        <v>0.94073353062204002</v>
+      </c>
+      <c r="M2" s="10">
+        <v>0.94138897123946497</v>
+      </c>
+      <c r="N2" s="10">
+        <v>0.94112983299960995</v>
+      </c>
+      <c r="O2" s="10">
+        <v>2.8461799105585498E-4</v>
+      </c>
+      <c r="P2" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>19</v>
+      </c>
+      <c r="B3" s="10">
+        <v>535.21947296460496</v>
+      </c>
+      <c r="C3" s="10">
+        <v>0.76695164687294404</v>
+      </c>
+      <c r="D3" s="10">
+        <v>0.36441365877787302</v>
+      </c>
+      <c r="E3" s="10">
+        <v>2.7845021590755799E-3</v>
+      </c>
+      <c r="F3" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G3" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I3" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="K3" s="10">
+        <v>0.94126699713732398</v>
+      </c>
+      <c r="L3" s="10">
+        <v>0.94073353062204002</v>
+      </c>
+      <c r="M3" s="10">
+        <v>0.94138897123946497</v>
+      </c>
+      <c r="N3" s="10">
+        <v>0.94112983299960995</v>
+      </c>
+      <c r="O3" s="10">
+        <v>2.8461799105585498E-4</v>
+      </c>
+      <c r="P3" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
+        <v>20</v>
+      </c>
+      <c r="B4" s="10">
+        <v>535.733668327332</v>
+      </c>
+      <c r="C4" s="10">
+        <v>0.66221849864691795</v>
+      </c>
+      <c r="D4" s="10">
+        <v>0.372064272562663</v>
+      </c>
+      <c r="E4" s="10">
+        <v>5.4894231709915501E-3</v>
+      </c>
+      <c r="F4" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G4" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H4" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I4" s="10">
+        <v>1</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="K4" s="10">
+        <v>0.94126699713732398</v>
+      </c>
+      <c r="L4" s="10">
+        <v>0.94073353062204002</v>
+      </c>
+      <c r="M4" s="10">
+        <v>0.94138897123946497</v>
+      </c>
+      <c r="N4" s="10">
+        <v>0.94112983299960995</v>
+      </c>
+      <c r="O4" s="10">
+        <v>2.8461799105585498E-4</v>
+      </c>
+      <c r="P4" s="10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A5" s="9">
+        <v>15</v>
+      </c>
+      <c r="B5" s="10">
+        <v>252.10780707995099</v>
+      </c>
+      <c r="C5" s="10">
+        <v>0.43373286411739598</v>
+      </c>
+      <c r="D5" s="10">
+        <v>0.25657622019449899</v>
+      </c>
+      <c r="E5" s="10">
+        <v>8.8768455208140598E-3</v>
+      </c>
+      <c r="F5" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G5" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H5" s="10">
+        <v>1</v>
+      </c>
+      <c r="I5" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J5" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="K5" s="10">
+        <v>0.93991219968252404</v>
+      </c>
+      <c r="L5" s="10">
+        <v>0.94064340252575596</v>
+      </c>
+      <c r="M5" s="10">
+        <v>0.94000728072520101</v>
+      </c>
+      <c r="N5" s="10">
+        <v>0.94018762764449404</v>
+      </c>
+      <c r="O5" s="10">
+        <v>3.2461069807917202E-4</v>
+      </c>
+      <c r="P5" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A6" s="9">
+        <v>16</v>
+      </c>
+      <c r="B6" s="10">
+        <v>251.945256312688</v>
+      </c>
+      <c r="C6" s="10">
+        <v>0.35612199703071901</v>
+      </c>
+      <c r="D6" s="10">
+        <v>0.25618775685628298</v>
+      </c>
+      <c r="E6" s="10">
+        <v>5.0539780819444501E-3</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G6" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H6" s="10">
+        <v>1</v>
+      </c>
+      <c r="I6" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="10" t="s">
+        <v>73</v>
+      </c>
+      <c r="K6" s="10">
+        <v>0.93991219968252404</v>
+      </c>
+      <c r="L6" s="10">
+        <v>0.94064340252575596</v>
+      </c>
+      <c r="M6" s="10">
+        <v>0.94000728072520101</v>
+      </c>
+      <c r="N6" s="10">
+        <v>0.94018762764449404</v>
+      </c>
+      <c r="O6" s="10">
+        <v>3.2461069807917202E-4</v>
+      </c>
+      <c r="P6" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A7" s="9">
+        <v>17</v>
+      </c>
+      <c r="B7" s="10">
+        <v>251.590544382731</v>
+      </c>
+      <c r="C7" s="10">
+        <v>0.38815126099478497</v>
+      </c>
+      <c r="D7" s="10">
+        <v>0.25162053108215299</v>
+      </c>
+      <c r="E7" s="10">
+        <v>3.9393946532317401E-3</v>
+      </c>
+      <c r="F7" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H7" s="10">
+        <v>1</v>
+      </c>
+      <c r="I7" s="10">
+        <v>1</v>
+      </c>
+      <c r="J7" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="K7" s="10">
+        <v>0.93991219968252404</v>
+      </c>
+      <c r="L7" s="10">
+        <v>0.94064340252575596</v>
+      </c>
+      <c r="M7" s="10">
+        <v>0.94000728072520101</v>
+      </c>
+      <c r="N7" s="10">
+        <v>0.94018762764449404</v>
+      </c>
+      <c r="O7" s="10">
+        <v>3.2461069807917202E-4</v>
+      </c>
+      <c r="P7" s="10">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A8" s="9">
+        <v>24</v>
+      </c>
+      <c r="B8" s="10">
+        <v>557.84657303492202</v>
+      </c>
+      <c r="C8" s="10">
+        <v>0.35076464356121101</v>
+      </c>
+      <c r="D8" s="10">
+        <v>0.37836964925130201</v>
+      </c>
+      <c r="E8" s="10">
+        <v>1.65763708530314E-3</v>
+      </c>
+      <c r="F8" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H8" s="10">
+        <v>1</v>
+      </c>
+      <c r="I8" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="K8" s="10">
+        <v>0.93973359815380597</v>
+      </c>
+      <c r="L8" s="10">
+        <v>0.94040154534127596</v>
+      </c>
+      <c r="M8" s="10">
+        <v>0.93995696507054005</v>
+      </c>
+      <c r="N8" s="10">
+        <v>0.94003070285520696</v>
+      </c>
+      <c r="O8" s="10">
+        <v>2.7762841710717202E-4</v>
+      </c>
+      <c r="P8" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A9" s="9">
+        <v>25</v>
+      </c>
+      <c r="B9" s="10">
+        <v>557.17929259936</v>
+      </c>
+      <c r="C9" s="10">
+        <v>0.40358160818365502</v>
+      </c>
+      <c r="D9" s="10">
+        <v>0.37869993845621702</v>
+      </c>
+      <c r="E9" s="10">
+        <v>3.9739786054019798E-3</v>
+      </c>
+      <c r="F9" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H9" s="10">
+        <v>1</v>
+      </c>
+      <c r="I9" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="K9" s="10">
+        <v>0.93973359815380597</v>
+      </c>
+      <c r="L9" s="10">
+        <v>0.94040154534127596</v>
+      </c>
+      <c r="M9" s="10">
+        <v>0.93995696507054005</v>
+      </c>
+      <c r="N9" s="10">
+        <v>0.94003070285520696</v>
+      </c>
+      <c r="O9" s="10">
+        <v>2.7762841710717202E-4</v>
+      </c>
+      <c r="P9" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A10" s="9">
+        <v>26</v>
+      </c>
+      <c r="B10" s="10">
+        <v>557.92489441235898</v>
+      </c>
+      <c r="C10" s="10">
+        <v>0.141467807989894</v>
+      </c>
+      <c r="D10" s="10">
+        <v>0.37772536277771002</v>
+      </c>
+      <c r="E10" s="10">
+        <v>5.7379239670770597E-3</v>
+      </c>
+      <c r="F10" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G10" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H10" s="10">
+        <v>1</v>
+      </c>
+      <c r="I10" s="10">
+        <v>1</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>84</v>
+      </c>
+      <c r="K10" s="10">
+        <v>0.93973359815380597</v>
+      </c>
+      <c r="L10" s="10">
+        <v>0.94040154534127596</v>
+      </c>
+      <c r="M10" s="10">
+        <v>0.93995696507054005</v>
+      </c>
+      <c r="N10" s="10">
+        <v>0.94003070285520696</v>
+      </c>
+      <c r="O10" s="10">
+        <v>2.7762841710717202E-4</v>
+      </c>
+      <c r="P10" s="10">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A11" s="9">
+        <v>21</v>
+      </c>
+      <c r="B11" s="10">
+        <v>536.93935378392496</v>
+      </c>
+      <c r="C11" s="10">
+        <v>3.5182234886644399</v>
+      </c>
+      <c r="D11" s="10">
+        <v>0.373094956080119</v>
+      </c>
+      <c r="E11" s="10">
+        <v>1.16992979366449E-2</v>
+      </c>
+      <c r="F11" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G11" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H11" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I11" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J11" s="10" t="s">
+        <v>79</v>
+      </c>
+      <c r="K11" s="10">
+        <v>0.93811408237452898</v>
+      </c>
+      <c r="L11" s="10">
+        <v>0.94254566312580401</v>
+      </c>
+      <c r="M11" s="10">
+        <v>0.93871673058723104</v>
+      </c>
+      <c r="N11" s="10">
+        <v>0.93979215869585497</v>
+      </c>
+      <c r="O11" s="10">
+        <v>1.9625045564925698E-3</v>
+      </c>
+      <c r="P11" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A12" s="9">
+        <v>22</v>
+      </c>
+      <c r="B12" s="10">
+        <v>557.65626414616895</v>
+      </c>
+      <c r="C12" s="10">
+        <v>0.19413253271817399</v>
+      </c>
+      <c r="D12" s="10">
+        <v>0.377368291219076</v>
+      </c>
+      <c r="E12" s="10">
+        <v>5.6333060091033399E-3</v>
+      </c>
+      <c r="F12" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I12" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J12" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="K12" s="10">
+        <v>0.93811408237452898</v>
+      </c>
+      <c r="L12" s="10">
+        <v>0.94254566312580401</v>
+      </c>
+      <c r="M12" s="10">
+        <v>0.93871673058723104</v>
+      </c>
+      <c r="N12" s="10">
+        <v>0.93979215869585497</v>
+      </c>
+      <c r="O12" s="10">
+        <v>1.9625045564925698E-3</v>
+      </c>
+      <c r="P12" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A13" s="9">
+        <v>23</v>
+      </c>
+      <c r="B13" s="10">
+        <v>558.23829833666503</v>
+      </c>
+      <c r="C13" s="10">
+        <v>0.21642645026792801</v>
+      </c>
+      <c r="D13" s="10">
+        <v>0.37876828511555999</v>
+      </c>
+      <c r="E13" s="10">
+        <v>1.78782910022144E-3</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G13" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H13" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I13" s="10">
+        <v>1</v>
+      </c>
+      <c r="J13" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="K13" s="10">
+        <v>0.93811408237452898</v>
+      </c>
+      <c r="L13" s="10">
+        <v>0.94254566312580401</v>
+      </c>
+      <c r="M13" s="10">
+        <v>0.93871673058723104</v>
+      </c>
+      <c r="N13" s="10">
+        <v>0.93979215869585497</v>
+      </c>
+      <c r="O13" s="10">
+        <v>1.9625045564925698E-3</v>
+      </c>
+      <c r="P13" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A14" s="9">
+        <v>12</v>
+      </c>
+      <c r="B14" s="10">
+        <v>251.44035482406599</v>
+      </c>
+      <c r="C14" s="10">
+        <v>0.42036134002939302</v>
+      </c>
+      <c r="D14" s="10">
+        <v>0.254356225331624</v>
+      </c>
+      <c r="E14" s="10">
+        <v>3.2236883180735399E-3</v>
+      </c>
+      <c r="F14" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G14" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H14" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I14" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J14" s="10" t="s">
+        <v>69</v>
+      </c>
+      <c r="K14" s="10">
+        <v>0.93936676587008405</v>
+      </c>
+      <c r="L14" s="10">
+        <v>0.94144935673387198</v>
+      </c>
+      <c r="M14" s="10">
+        <v>0.93834214179938502</v>
+      </c>
+      <c r="N14" s="10">
+        <v>0.93971942146777998</v>
+      </c>
+      <c r="O14" s="10">
+        <v>1.2927930074625299E-3</v>
+      </c>
+      <c r="P14" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A15" s="9">
+        <v>13</v>
+      </c>
+      <c r="B15" s="10">
+        <v>251.55283466974899</v>
+      </c>
+      <c r="C15" s="10">
+        <v>0.146535456617332</v>
+      </c>
+      <c r="D15" s="10">
+        <v>0.24670100212097201</v>
+      </c>
+      <c r="E15" s="10">
+        <v>3.9726725808011901E-3</v>
+      </c>
+      <c r="F15" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G15" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H15" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I15" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="10">
+        <v>0.93936676587008405</v>
+      </c>
+      <c r="L15" s="10">
+        <v>0.94144935673387198</v>
+      </c>
+      <c r="M15" s="10">
+        <v>0.93834214179938502</v>
+      </c>
+      <c r="N15" s="10">
+        <v>0.93971942146777998</v>
+      </c>
+      <c r="O15" s="10">
+        <v>1.2927930074625299E-3</v>
+      </c>
+      <c r="P15" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A16" s="9">
+        <v>14</v>
+      </c>
+      <c r="B16" s="10">
+        <v>252.05603273709599</v>
+      </c>
+      <c r="C16" s="10">
+        <v>0.155872308003563</v>
+      </c>
+      <c r="D16" s="10">
+        <v>0.25334795316060399</v>
+      </c>
+      <c r="E16" s="10">
+        <v>4.2833312379272999E-3</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G16" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H16" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I16" s="10">
+        <v>1</v>
+      </c>
+      <c r="J16" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="K16" s="10">
+        <v>0.93936676587008405</v>
+      </c>
+      <c r="L16" s="10">
+        <v>0.94144935673387198</v>
+      </c>
+      <c r="M16" s="10">
+        <v>0.93834214179938502</v>
+      </c>
+      <c r="N16" s="10">
+        <v>0.93971942146777998</v>
+      </c>
+      <c r="O16" s="10">
+        <v>1.2927930074625299E-3</v>
+      </c>
+      <c r="P16" s="10">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A17" s="9">
+        <v>9</v>
+      </c>
+      <c r="B17" s="10">
+        <v>259.94605755805998</v>
+      </c>
+      <c r="C17" s="10">
+        <v>2.2401125226944298</v>
+      </c>
+      <c r="D17" s="10">
+        <v>0.24852315584818499</v>
+      </c>
+      <c r="E17" s="10">
+        <v>6.1038274031388401E-4</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G17" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H17" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I17" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J17" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="K17" s="10">
+        <v>0.93812634410037199</v>
+      </c>
+      <c r="L17" s="10">
+        <v>0.94163757179090102</v>
+      </c>
+      <c r="M17" s="10">
+        <v>0.93828982182241005</v>
+      </c>
+      <c r="N17" s="10">
+        <v>0.93935124590456098</v>
+      </c>
+      <c r="O17" s="10">
+        <v>1.61805351895636E-3</v>
+      </c>
+      <c r="P17" s="10">
+        <v>16</v>
+      </c>
+      <c r="R17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A18" s="9">
+        <v>10</v>
+      </c>
+      <c r="B18" s="10">
+        <v>255.603337605794</v>
+      </c>
+      <c r="C18" s="10">
+        <v>2.1750142871537501</v>
+      </c>
+      <c r="D18" s="10">
+        <v>0.25511741638183599</v>
+      </c>
+      <c r="E18" s="10">
+        <v>7.57071521690297E-3</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H18" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I18" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J18" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0.93812634410037199</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0.94163757179090102</v>
+      </c>
+      <c r="M18" s="10">
+        <v>0.93828982182241005</v>
+      </c>
+      <c r="N18" s="10">
+        <v>0.93935124590456098</v>
+      </c>
+      <c r="O18" s="10">
+        <v>1.61805351895636E-3</v>
+      </c>
+      <c r="P18" s="10">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A19" s="9">
+        <v>11</v>
+      </c>
+      <c r="B19" s="10">
+        <v>252.42304595311501</v>
+      </c>
+      <c r="C19" s="10">
+        <v>0.49374621291668302</v>
+      </c>
+      <c r="D19" s="10">
+        <v>0.25171343485514303</v>
+      </c>
+      <c r="E19" s="10">
+        <v>2.3784159568269198E-3</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G19" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H19" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I19" s="10">
+        <v>1</v>
+      </c>
+      <c r="J19" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="K19" s="10">
+        <v>0.93812634410037199</v>
+      </c>
+      <c r="L19" s="10">
+        <v>0.94163757179090102</v>
+      </c>
+      <c r="M19" s="10">
+        <v>0.93828982182241005</v>
+      </c>
+      <c r="N19" s="10">
+        <v>0.93935124590456098</v>
+      </c>
+      <c r="O19" s="10">
+        <v>1.61805351895636E-3</v>
+      </c>
+      <c r="P19" s="10">
+        <v>16</v>
+      </c>
+      <c r="R19">
+        <f>30145.05/60/60</f>
+        <v>8.3736249999999988</v>
+      </c>
+      <c r="S19" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A20" s="9">
+        <v>0</v>
+      </c>
+      <c r="B20" s="10">
+        <v>7.9298910299936898</v>
+      </c>
+      <c r="C20" s="10">
+        <v>3.03060846140855</v>
+      </c>
+      <c r="D20" s="10">
+        <v>0.132151047388713</v>
+      </c>
+      <c r="E20" s="10">
+        <v>3.4594786367977701E-3</v>
+      </c>
+      <c r="F20" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G20" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H20" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I20" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>56</v>
+      </c>
+      <c r="K20" s="10">
+        <v>0.91425022042003801</v>
+      </c>
+      <c r="L20" s="10">
+        <v>0.91341544886999504</v>
+      </c>
+      <c r="M20" s="10">
+        <v>0.91462773737535996</v>
+      </c>
+      <c r="N20" s="10">
+        <v>0.91409780222179804</v>
+      </c>
+      <c r="O20" s="10">
+        <v>5.0651379410412403E-4</v>
+      </c>
+      <c r="P20" s="10">
+        <v>19</v>
+      </c>
+      <c r="R20" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A21" s="9">
+        <v>1</v>
+      </c>
+      <c r="B21" s="10">
+        <v>7.4722809791564897</v>
+      </c>
+      <c r="C21" s="10">
+        <v>1.65225362674015</v>
+      </c>
+      <c r="D21" s="10">
+        <v>0.145226240158081</v>
+      </c>
+      <c r="E21" s="10">
+        <v>1.38757707682699E-2</v>
+      </c>
+      <c r="F21" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H21" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I21" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J21" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="K21" s="10">
+        <v>0.91425022042003801</v>
+      </c>
+      <c r="L21" s="10">
+        <v>0.91341544886999504</v>
+      </c>
+      <c r="M21" s="10">
+        <v>0.91462773737535996</v>
+      </c>
+      <c r="N21" s="10">
+        <v>0.91409780222179804</v>
+      </c>
+      <c r="O21" s="10">
+        <v>5.0651379410412403E-4</v>
+      </c>
+      <c r="P21" s="10">
+        <v>19</v>
+      </c>
+      <c r="R21" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A22" s="9">
+        <v>2</v>
+      </c>
+      <c r="B22" s="10">
+        <v>8.4732604026794398</v>
+      </c>
+      <c r="C22" s="10">
+        <v>2.6948055220034002</v>
+      </c>
+      <c r="D22" s="10">
+        <v>0.13473129272460899</v>
+      </c>
+      <c r="E22" s="10">
+        <v>1.9028042161123599E-3</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H22" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I22" s="10">
+        <v>1</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="K22" s="10">
+        <v>0.91425022042003801</v>
+      </c>
+      <c r="L22" s="10">
+        <v>0.91341544886999504</v>
+      </c>
+      <c r="M22" s="10">
+        <v>0.91462773737535996</v>
+      </c>
+      <c r="N22" s="10">
+        <v>0.91409780222179804</v>
+      </c>
+      <c r="O22" s="10">
+        <v>5.0651379410412403E-4</v>
+      </c>
+      <c r="P22" s="10">
+        <v>19</v>
+      </c>
+      <c r="R22" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A23" s="9">
+        <v>3</v>
+      </c>
+      <c r="B23" s="10">
+        <v>72.476766029993698</v>
+      </c>
+      <c r="C23" s="10">
+        <v>2.3409929889373302</v>
+      </c>
+      <c r="D23" s="10">
+        <v>0.13195935885111501</v>
+      </c>
+      <c r="E23" s="10">
+        <v>1.93526403846799E-3</v>
+      </c>
+      <c r="F23" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G23" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H23" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I23" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J23" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="K23" s="10">
+        <v>0.91212029320793797</v>
+      </c>
+      <c r="L23" s="10">
+        <v>0.912630659232745</v>
+      </c>
+      <c r="M23" s="10">
+        <v>0.90793500556700701</v>
+      </c>
+      <c r="N23" s="10">
+        <v>0.91089531933589696</v>
+      </c>
+      <c r="O23" s="10">
+        <v>2.10360192329363E-3</v>
+      </c>
+      <c r="P23" s="10">
+        <v>22</v>
+      </c>
+      <c r="R23" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A24" s="9">
+        <v>4</v>
+      </c>
+      <c r="B24" s="10">
+        <v>72.093354384104401</v>
+      </c>
+      <c r="C24" s="10">
+        <v>0.538082050260974</v>
+      </c>
+      <c r="D24" s="10">
+        <v>0.133479277292887</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1.6706106753568001E-3</v>
+      </c>
+      <c r="F24" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H24" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I24" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J24" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="K24" s="10">
+        <v>0.91212029320793797</v>
+      </c>
+      <c r="L24" s="10">
+        <v>0.912630659232745</v>
+      </c>
+      <c r="M24" s="10">
+        <v>0.90793500556700701</v>
+      </c>
+      <c r="N24" s="10">
+        <v>0.91089531933589696</v>
+      </c>
+      <c r="O24" s="10">
+        <v>2.10360192329363E-3</v>
+      </c>
+      <c r="P24" s="10">
+        <v>22</v>
+      </c>
+      <c r="R24" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A25" s="9">
+        <v>5</v>
+      </c>
+      <c r="B25" s="10">
+        <v>72.835770368576107</v>
+      </c>
+      <c r="C25" s="10">
+        <v>0.261224246609293</v>
+      </c>
+      <c r="D25" s="10">
+        <v>0.13378826777140301</v>
+      </c>
+      <c r="E25" s="10">
+        <v>1.76077143832002E-3</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H25" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I25" s="10">
+        <v>1</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>61</v>
+      </c>
+      <c r="K25" s="10">
+        <v>0.91212029320793797</v>
+      </c>
+      <c r="L25" s="10">
+        <v>0.912630659232745</v>
+      </c>
+      <c r="M25" s="10">
+        <v>0.90793500556700701</v>
+      </c>
+      <c r="N25" s="10">
+        <v>0.91089531933589696</v>
+      </c>
+      <c r="O25" s="10">
+        <v>2.10360192329363E-3</v>
+      </c>
+      <c r="P25" s="10">
+        <v>22</v>
+      </c>
+      <c r="R25" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A26" s="9">
+        <v>27</v>
+      </c>
+      <c r="B26" s="10">
+        <v>5.2542745272318498</v>
+      </c>
+      <c r="C26" s="10">
+        <v>0.150327403005343</v>
+      </c>
+      <c r="D26" s="10">
+        <v>0.16156967480977399</v>
+      </c>
+      <c r="E26" s="10">
+        <v>3.8716717880995801E-3</v>
+      </c>
+      <c r="F26" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G26" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H26" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I26" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>86</v>
+      </c>
+      <c r="K26" s="10">
+        <v>0.91069573523908098</v>
+      </c>
+      <c r="L26" s="10">
+        <v>0.91283968501926205</v>
+      </c>
+      <c r="M26" s="10">
+        <v>0.90641756437979304</v>
+      </c>
+      <c r="N26" s="10">
+        <v>0.90998432821271202</v>
+      </c>
+      <c r="O26" s="10">
+        <v>2.6696420914732E-3</v>
+      </c>
+      <c r="P26" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A27" s="9">
+        <v>28</v>
+      </c>
+      <c r="B27" s="10">
+        <v>5.25998854637146</v>
+      </c>
+      <c r="C27" s="10">
+        <v>9.4053630853889403E-2</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0.15441711743672701</v>
+      </c>
+      <c r="E27" s="10">
+        <v>5.5218741651853701E-3</v>
+      </c>
+      <c r="F27" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G27" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H27" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J27" s="10" t="s">
+        <v>87</v>
+      </c>
+      <c r="K27" s="10">
+        <v>0.91069573523908098</v>
+      </c>
+      <c r="L27" s="10">
+        <v>0.91283968501926205</v>
+      </c>
+      <c r="M27" s="10">
+        <v>0.90641756437979304</v>
+      </c>
+      <c r="N27" s="10">
+        <v>0.90998432821271202</v>
+      </c>
+      <c r="O27" s="10">
+        <v>2.6696420914732E-3</v>
+      </c>
+      <c r="P27" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A28" s="9">
+        <v>29</v>
+      </c>
+      <c r="B28" s="10">
+        <v>5.0566283067067497</v>
+      </c>
+      <c r="C28" s="10">
+        <v>3.0223203587596901E-3</v>
+      </c>
+      <c r="D28" s="10">
+        <v>0.149218718210856</v>
+      </c>
+      <c r="E28" s="10">
+        <v>1.9682312901134198E-3</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G28" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I28" s="10">
+        <v>1</v>
+      </c>
+      <c r="J28" s="10" t="s">
+        <v>88</v>
+      </c>
+      <c r="K28" s="10">
+        <v>0.91069573523908098</v>
+      </c>
+      <c r="L28" s="10">
+        <v>0.91283968501926205</v>
+      </c>
+      <c r="M28" s="10">
+        <v>0.90641756437979304</v>
+      </c>
+      <c r="N28" s="10">
+        <v>0.90998432821271202</v>
+      </c>
+      <c r="O28" s="10">
+        <v>2.6696420914732E-3</v>
+      </c>
+      <c r="P28" s="10">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="29" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A29" s="9">
+        <v>45</v>
+      </c>
+      <c r="B29" s="10">
+        <v>38.275189399719203</v>
+      </c>
+      <c r="C29" s="10">
+        <v>6.5381589857861105E-2</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0.4676407178243</v>
+      </c>
+      <c r="E29" s="10">
+        <v>3.8388100933869798E-3</v>
+      </c>
+      <c r="F29" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H29" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I29" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J29" s="10" t="s">
+        <v>104</v>
+      </c>
+      <c r="K29" s="10">
+        <v>0.90342417310936296</v>
+      </c>
+      <c r="L29" s="10">
+        <v>0.91626223546493502</v>
+      </c>
+      <c r="M29" s="10">
+        <v>0.91016013596088197</v>
+      </c>
+      <c r="N29" s="10">
+        <v>0.90994884817839305</v>
+      </c>
+      <c r="O29" s="10">
+        <v>5.24324601474189E-3</v>
+      </c>
+      <c r="P29" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A30" s="9">
+        <v>46</v>
+      </c>
+      <c r="B30" s="10">
+        <v>38.321452220281003</v>
+      </c>
+      <c r="C30" s="10">
+        <v>0.24718966012971699</v>
+      </c>
+      <c r="D30" s="10">
+        <v>0.46366429328918501</v>
+      </c>
+      <c r="E30" s="10">
+        <v>8.6058142999279903E-3</v>
+      </c>
+      <c r="F30" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G30" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H30" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I30" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J30" s="10" t="s">
+        <v>105</v>
+      </c>
+      <c r="K30" s="10">
+        <v>0.90342417310936296</v>
+      </c>
+      <c r="L30" s="10">
+        <v>0.91626223546493502</v>
+      </c>
+      <c r="M30" s="10">
+        <v>0.91016013596088197</v>
+      </c>
+      <c r="N30" s="10">
+        <v>0.90994884817839305</v>
+      </c>
+      <c r="O30" s="10">
+        <v>5.24324601474189E-3</v>
+      </c>
+      <c r="P30" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A31" s="9">
+        <v>47</v>
+      </c>
+      <c r="B31" s="10">
+        <v>38.308750708897897</v>
+      </c>
+      <c r="C31" s="10">
+        <v>0.20797803791091499</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0.45550068219502798</v>
+      </c>
+      <c r="E31" s="10">
+        <v>3.81889365932904E-3</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G31" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H31" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I31" s="10">
+        <v>1</v>
+      </c>
+      <c r="J31" s="10" t="s">
+        <v>106</v>
+      </c>
+      <c r="K31" s="10">
+        <v>0.90342417310936296</v>
+      </c>
+      <c r="L31" s="10">
+        <v>0.91626223546493502</v>
+      </c>
+      <c r="M31" s="10">
+        <v>0.91016013596088197</v>
+      </c>
+      <c r="N31" s="10">
+        <v>0.90994884817839305</v>
+      </c>
+      <c r="O31" s="10">
+        <v>5.24324601474189E-3</v>
+      </c>
+      <c r="P31" s="10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="32" spans="1:19" x14ac:dyDescent="0.2">
+      <c r="A32" s="9">
+        <v>36</v>
+      </c>
+      <c r="B32" s="10">
+        <v>18.391877333323201</v>
+      </c>
+      <c r="C32" s="10">
+        <v>0.25915130647689499</v>
+      </c>
+      <c r="D32" s="10">
+        <v>0.29879204432169598</v>
+      </c>
+      <c r="E32" s="10">
+        <v>5.95220578987258E-3</v>
+      </c>
+      <c r="F32" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G32" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H32" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I32" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J32" s="10" t="s">
+        <v>95</v>
+      </c>
+      <c r="K32" s="10">
+        <v>0.90343646795166399</v>
+      </c>
+      <c r="L32" s="10">
+        <v>0.90692469525377095</v>
+      </c>
+      <c r="M32" s="10">
+        <v>0.90841208854183397</v>
+      </c>
+      <c r="N32" s="10">
+        <v>0.90625775058242297</v>
+      </c>
+      <c r="O32" s="10">
+        <v>2.0853155573053602E-3</v>
+      </c>
+      <c r="P32" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A33" s="9">
+        <v>37</v>
+      </c>
+      <c r="B33" s="10">
+        <v>18.538251320520999</v>
+      </c>
+      <c r="C33" s="10">
+        <v>0.19422131376134799</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0.29914697011311803</v>
+      </c>
+      <c r="E33" s="10">
+        <v>9.0110089423252292E-3</v>
+      </c>
+      <c r="F33" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G33" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I33" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J33" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="K33" s="10">
+        <v>0.90343646795166399</v>
+      </c>
+      <c r="L33" s="10">
+        <v>0.90692469525377095</v>
+      </c>
+      <c r="M33" s="10">
+        <v>0.90841208854183397</v>
+      </c>
+      <c r="N33" s="10">
+        <v>0.90625775058242297</v>
+      </c>
+      <c r="O33" s="10">
+        <v>2.0853155573053602E-3</v>
+      </c>
+      <c r="P33" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A34" s="9">
+        <v>38</v>
+      </c>
+      <c r="B34" s="10">
+        <v>18.793636322021499</v>
+      </c>
+      <c r="C34" s="10">
+        <v>0.26761471130508202</v>
+      </c>
+      <c r="D34" s="10">
+        <v>0.29939397176106802</v>
+      </c>
+      <c r="E34" s="10">
+        <v>2.8579427863298801E-3</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H34" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="I34" s="10">
+        <v>1</v>
+      </c>
+      <c r="J34" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K34" s="10">
+        <v>0.90343646795166399</v>
+      </c>
+      <c r="L34" s="10">
+        <v>0.90692469525377095</v>
+      </c>
+      <c r="M34" s="10">
+        <v>0.90841208854183397</v>
+      </c>
+      <c r="N34" s="10">
+        <v>0.90625775058242297</v>
+      </c>
+      <c r="O34" s="10">
+        <v>2.0853155573053602E-3</v>
+      </c>
+      <c r="P34" s="10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A35" s="9">
+        <v>51</v>
+      </c>
+      <c r="B35" s="10">
+        <v>559.95782971382096</v>
+      </c>
+      <c r="C35" s="10">
+        <v>0.63258157804511295</v>
+      </c>
+      <c r="D35" s="10">
+        <v>0.40350270271301297</v>
+      </c>
+      <c r="E35" s="10">
+        <v>7.0479008152994202E-3</v>
+      </c>
+      <c r="F35" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G35" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H35" s="10">
+        <v>1</v>
+      </c>
+      <c r="I35" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J35" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="K35" s="10">
+        <v>0.90559945125444596</v>
+      </c>
+      <c r="L35" s="10">
+        <v>0.90390870222068498</v>
+      </c>
+      <c r="M35" s="10">
+        <v>0.90243108256105398</v>
+      </c>
+      <c r="N35" s="10">
+        <v>0.90397974534539505</v>
+      </c>
+      <c r="O35" s="10">
+        <v>1.2944562277891201E-3</v>
+      </c>
+      <c r="P35" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A36" s="9">
+        <v>52</v>
+      </c>
+      <c r="B36" s="10">
+        <v>559.19372034072899</v>
+      </c>
+      <c r="C36" s="10">
+        <v>1.24034322456377</v>
+      </c>
+      <c r="D36" s="10">
+        <v>0.40301632881164601</v>
+      </c>
+      <c r="E36" s="10">
+        <v>2.3594593307434799E-3</v>
+      </c>
+      <c r="F36" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G36" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H36" s="10">
+        <v>1</v>
+      </c>
+      <c r="I36" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J36" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="K36" s="10">
+        <v>0.90559945125444596</v>
+      </c>
+      <c r="L36" s="10">
+        <v>0.90390870222068498</v>
+      </c>
+      <c r="M36" s="10">
+        <v>0.90243108256105398</v>
+      </c>
+      <c r="N36" s="10">
+        <v>0.90397974534539505</v>
+      </c>
+      <c r="O36" s="10">
+        <v>1.2944562277891201E-3</v>
+      </c>
+      <c r="P36" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A37" s="9">
+        <v>53</v>
+      </c>
+      <c r="B37" s="10">
+        <v>562.48345843950904</v>
+      </c>
+      <c r="C37" s="10">
+        <v>4.1233715383574303</v>
+      </c>
+      <c r="D37" s="10">
+        <v>0.402181069056193</v>
+      </c>
+      <c r="E37" s="10">
+        <v>5.5474011399038702E-3</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G37" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H37" s="10">
+        <v>1</v>
+      </c>
+      <c r="I37" s="10">
+        <v>1</v>
+      </c>
+      <c r="J37" s="10" t="s">
+        <v>112</v>
+      </c>
+      <c r="K37" s="10">
+        <v>0.90559945125444596</v>
+      </c>
+      <c r="L37" s="10">
+        <v>0.90390870222068498</v>
+      </c>
+      <c r="M37" s="10">
+        <v>0.90243108256105398</v>
+      </c>
+      <c r="N37" s="10">
+        <v>0.90397974534539505</v>
+      </c>
+      <c r="O37" s="10">
+        <v>1.2944562277891201E-3</v>
+      </c>
+      <c r="P37" s="10">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A38" s="9">
+        <v>48</v>
+      </c>
+      <c r="B38" s="10">
+        <v>34.234447240829503</v>
+      </c>
+      <c r="C38" s="10">
+        <v>0.26926235839379797</v>
+      </c>
+      <c r="D38" s="10">
+        <v>0.41066431999206499</v>
+      </c>
+      <c r="E38" s="10">
+        <v>1.4227727341120299E-3</v>
+      </c>
+      <c r="F38" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G38" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H38" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I38" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J38" s="10" t="s">
+        <v>107</v>
+      </c>
+      <c r="K38" s="10">
+        <v>0.89736925055771799</v>
+      </c>
+      <c r="L38" s="10">
+        <v>0.90323335821148498</v>
+      </c>
+      <c r="M38" s="10">
+        <v>0.904485066254331</v>
+      </c>
+      <c r="N38" s="10">
+        <v>0.90169589167451103</v>
+      </c>
+      <c r="O38" s="10">
+        <v>3.10178021693758E-3</v>
+      </c>
+      <c r="P38" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A39" s="9">
+        <v>49</v>
+      </c>
+      <c r="B39" s="10">
+        <v>34.134116013844803</v>
+      </c>
+      <c r="C39" s="10">
+        <v>2.1800087775719301E-2</v>
+      </c>
+      <c r="D39" s="10">
+        <v>0.40955265363057503</v>
+      </c>
+      <c r="E39" s="10">
+        <v>4.3569098718476704E-3</v>
+      </c>
+      <c r="F39" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G39" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H39" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I39" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J39" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="K39" s="10">
+        <v>0.89736925055771799</v>
+      </c>
+      <c r="L39" s="10">
+        <v>0.90323335821148498</v>
+      </c>
+      <c r="M39" s="10">
+        <v>0.904485066254331</v>
+      </c>
+      <c r="N39" s="10">
+        <v>0.90169589167451103</v>
+      </c>
+      <c r="O39" s="10">
+        <v>3.10178021693758E-3</v>
+      </c>
+      <c r="P39" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A40" s="9">
+        <v>50</v>
+      </c>
+      <c r="B40" s="10">
+        <v>34.2665876547496</v>
+      </c>
+      <c r="C40" s="10">
+        <v>0.14678581764778001</v>
+      </c>
+      <c r="D40" s="10">
+        <v>0.40592058499654099</v>
+      </c>
+      <c r="E40" s="10">
+        <v>5.9756030583587802E-4</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G40" s="10" t="s">
+        <v>75</v>
+      </c>
+      <c r="H40" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I40" s="10">
+        <v>1</v>
+      </c>
+      <c r="J40" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="K40" s="10">
+        <v>0.89736925055771799</v>
+      </c>
+      <c r="L40" s="10">
+        <v>0.90323335821148498</v>
+      </c>
+      <c r="M40" s="10">
+        <v>0.904485066254331</v>
+      </c>
+      <c r="N40" s="10">
+        <v>0.90169589167451103</v>
+      </c>
+      <c r="O40" s="10">
+        <v>3.10178021693758E-3</v>
+      </c>
+      <c r="P40" s="10">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A41" s="9">
+        <v>39</v>
+      </c>
+      <c r="B41" s="10">
+        <v>16.3023447195689</v>
+      </c>
+      <c r="C41" s="10">
+        <v>4.8960852414779703E-2</v>
+      </c>
+      <c r="D41" s="10">
+        <v>0.27703992525736498</v>
+      </c>
+      <c r="E41" s="10">
+        <v>3.70476854763759E-3</v>
+      </c>
+      <c r="F41" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G41" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H41" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I41" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J41" s="10" t="s">
+        <v>98</v>
+      </c>
+      <c r="K41" s="10">
+        <v>0.89330994856928203</v>
+      </c>
+      <c r="L41" s="10">
+        <v>0.90206190858774804</v>
+      </c>
+      <c r="M41" s="10">
+        <v>0.90008256604847003</v>
+      </c>
+      <c r="N41" s="10">
+        <v>0.89848480773516604</v>
+      </c>
+      <c r="O41" s="10">
+        <v>3.7473390347467798E-3</v>
+      </c>
+      <c r="P41" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A42" s="9">
+        <v>40</v>
+      </c>
+      <c r="B42" s="10">
+        <v>16.3671193917592</v>
+      </c>
+      <c r="C42" s="10">
+        <v>7.9081127249900796E-2</v>
+      </c>
+      <c r="D42" s="10">
+        <v>0.27511938412984199</v>
+      </c>
+      <c r="E42" s="10">
+        <v>8.0705294950355905E-3</v>
+      </c>
+      <c r="F42" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G42" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H42" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I42" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J42" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="K42" s="10">
+        <v>0.89330994856928203</v>
+      </c>
+      <c r="L42" s="10">
+        <v>0.90206190858774804</v>
+      </c>
+      <c r="M42" s="10">
+        <v>0.90008256604847003</v>
+      </c>
+      <c r="N42" s="10">
+        <v>0.89848480773516604</v>
+      </c>
+      <c r="O42" s="10">
+        <v>3.7473390347467798E-3</v>
+      </c>
+      <c r="P42" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A43" s="9">
+        <v>41</v>
+      </c>
+      <c r="B43" s="10">
+        <v>16.316943009694398</v>
+      </c>
+      <c r="C43" s="10">
+        <v>6.1127465107720602E-2</v>
+      </c>
+      <c r="D43" s="10">
+        <v>0.26954229672749802</v>
+      </c>
+      <c r="E43" s="10">
+        <v>2.8758934145087E-3</v>
+      </c>
+      <c r="F43" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G43" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H43" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I43" s="10">
+        <v>1</v>
+      </c>
+      <c r="J43" s="10" t="s">
+        <v>100</v>
+      </c>
+      <c r="K43" s="10">
+        <v>0.89330994856928203</v>
+      </c>
+      <c r="L43" s="10">
+        <v>0.90206190858774804</v>
+      </c>
+      <c r="M43" s="10">
+        <v>0.90008256604847003</v>
+      </c>
+      <c r="N43" s="10">
+        <v>0.89848480773516604</v>
+      </c>
+      <c r="O43" s="10">
+        <v>3.7473390347467798E-3</v>
+      </c>
+      <c r="P43" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A44" s="9">
+        <v>42</v>
+      </c>
+      <c r="B44" s="10">
+        <v>16.729902744293199</v>
+      </c>
+      <c r="C44" s="10">
+        <v>0.54650381987210095</v>
+      </c>
+      <c r="D44" s="10">
+        <v>0.27282730738321898</v>
+      </c>
+      <c r="E44" s="10">
+        <v>1.7216202607015401E-3</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G44" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H44" s="10">
+        <v>1</v>
+      </c>
+      <c r="I44" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J44" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="K44" s="10">
+        <v>0.88904084892167101</v>
+      </c>
+      <c r="L44" s="10">
+        <v>0.90188516530856</v>
+      </c>
+      <c r="M44" s="10">
+        <v>0.90127360063735695</v>
+      </c>
+      <c r="N44" s="10">
+        <v>0.89739987162252899</v>
+      </c>
+      <c r="O44" s="10">
+        <v>5.9159923496607302E-3</v>
+      </c>
+      <c r="P44" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A45" s="9">
+        <v>43</v>
+      </c>
+      <c r="B45" s="10">
+        <v>16.805619398752899</v>
+      </c>
+      <c r="C45" s="10">
+        <v>0.55843102420105095</v>
+      </c>
+      <c r="D45" s="10">
+        <v>0.26975393295288103</v>
+      </c>
+      <c r="E45" s="10">
+        <v>5.5395025847536803E-3</v>
+      </c>
+      <c r="F45" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G45" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H45" s="10">
+        <v>1</v>
+      </c>
+      <c r="I45" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J45" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="K45" s="10">
+        <v>0.88904084892167101</v>
+      </c>
+      <c r="L45" s="10">
+        <v>0.90188516530856</v>
+      </c>
+      <c r="M45" s="10">
+        <v>0.90127360063735695</v>
+      </c>
+      <c r="N45" s="10">
+        <v>0.89739987162252899</v>
+      </c>
+      <c r="O45" s="10">
+        <v>5.9159923496607302E-3</v>
+      </c>
+      <c r="P45" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A46" s="9">
+        <v>44</v>
+      </c>
+      <c r="B46" s="10">
+        <v>16.776389678319301</v>
+      </c>
+      <c r="C46" s="10">
+        <v>0.62429874036194799</v>
+      </c>
+      <c r="D46" s="10">
+        <v>0.283157348632813</v>
+      </c>
+      <c r="E46" s="10">
+        <v>3.6014272200593899E-3</v>
+      </c>
+      <c r="F46" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G46" s="10" t="s">
+        <v>65</v>
+      </c>
+      <c r="H46" s="10">
+        <v>1</v>
+      </c>
+      <c r="I46" s="10">
+        <v>1</v>
+      </c>
+      <c r="J46" s="10" t="s">
+        <v>103</v>
+      </c>
+      <c r="K46" s="10">
+        <v>0.88904084892167101</v>
+      </c>
+      <c r="L46" s="10">
+        <v>0.90188516530856</v>
+      </c>
+      <c r="M46" s="10">
+        <v>0.90127360063735695</v>
+      </c>
+      <c r="N46" s="10">
+        <v>0.89739987162252899</v>
+      </c>
+      <c r="O46" s="10">
+        <v>5.9159923496607302E-3</v>
+      </c>
+      <c r="P46" s="10">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A47" s="9">
+        <v>30</v>
+      </c>
+      <c r="B47" s="10">
+        <v>4.4020232359568299</v>
+      </c>
+      <c r="C47" s="10">
+        <v>7.1834774724164899E-2</v>
+      </c>
+      <c r="D47" s="10">
+        <v>0.140361706415812</v>
+      </c>
+      <c r="E47" s="10">
+        <v>3.9928962999594003E-3</v>
+      </c>
+      <c r="F47" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G47" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H47" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I47" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J47" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="K47" s="10">
+        <v>0.89067079137900296</v>
+      </c>
+      <c r="L47" s="10">
+        <v>0.89338767026285804</v>
+      </c>
+      <c r="M47" s="10">
+        <v>0.89181996206432801</v>
+      </c>
+      <c r="N47" s="10">
+        <v>0.89195947456873004</v>
+      </c>
+      <c r="O47" s="10">
+        <v>1.1135395582098299E-3</v>
+      </c>
+      <c r="P47" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A48" s="9">
+        <v>31</v>
+      </c>
+      <c r="B48" s="10">
+        <v>4.4077916145324698</v>
+      </c>
+      <c r="C48" s="10">
+        <v>4.9325262367467801E-2</v>
+      </c>
+      <c r="D48" s="10">
+        <v>0.14140367507934601</v>
+      </c>
+      <c r="E48" s="10">
+        <v>2.0577758348681498E-3</v>
+      </c>
+      <c r="F48" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G48" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H48" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J48" s="10" t="s">
+        <v>90</v>
+      </c>
+      <c r="K48" s="10">
+        <v>0.89067079137900296</v>
+      </c>
+      <c r="L48" s="10">
+        <v>0.89338767026285804</v>
+      </c>
+      <c r="M48" s="10">
+        <v>0.89181996206432801</v>
+      </c>
+      <c r="N48" s="10">
+        <v>0.89195947456873004</v>
+      </c>
+      <c r="O48" s="10">
+        <v>1.1135395582098299E-3</v>
+      </c>
+      <c r="P48" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A49" s="9">
+        <v>32</v>
+      </c>
+      <c r="B49" s="10">
+        <v>4.5432793299357099</v>
+      </c>
+      <c r="C49" s="10">
+        <v>4.4963749086833503E-2</v>
+      </c>
+      <c r="D49" s="10">
+        <v>0.14638241132100399</v>
+      </c>
+      <c r="E49" s="10">
+        <v>4.7135778402265099E-3</v>
+      </c>
+      <c r="F49" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G49" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H49" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="I49" s="10">
+        <v>1</v>
+      </c>
+      <c r="J49" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="K49" s="10">
+        <v>0.89067079137900296</v>
+      </c>
+      <c r="L49" s="10">
+        <v>0.89338767026285804</v>
+      </c>
+      <c r="M49" s="10">
+        <v>0.89181996206432801</v>
+      </c>
+      <c r="N49" s="10">
+        <v>0.89195947456873004</v>
+      </c>
+      <c r="O49" s="10">
+        <v>1.1135395582098299E-3</v>
+      </c>
+      <c r="P49" s="10">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="50" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A50" s="9">
+        <v>6</v>
+      </c>
+      <c r="B50" s="10">
+        <v>73.400929927825899</v>
+      </c>
+      <c r="C50" s="10">
+        <v>8.8997084377555602E-2</v>
+      </c>
+      <c r="D50" s="10">
+        <v>0.14049736658732101</v>
+      </c>
+      <c r="E50" s="10">
+        <v>4.3890441812585602E-3</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G50" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H50" s="10">
+        <v>1</v>
+      </c>
+      <c r="I50" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J50" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="K50" s="10">
+        <v>0.87759036570541105</v>
+      </c>
+      <c r="L50" s="10">
+        <v>0.87840603275181495</v>
+      </c>
+      <c r="M50" s="10">
+        <v>0.90687510757939305</v>
+      </c>
+      <c r="N50" s="10">
+        <v>0.88762383534554001</v>
+      </c>
+      <c r="O50" s="10">
+        <v>1.3616777400180399E-2</v>
+      </c>
+      <c r="P50" s="10">
+        <v>49</v>
+      </c>
+      <c r="R50" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="51" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A51" s="9">
+        <v>7</v>
+      </c>
+      <c r="B51" s="10">
+        <v>73.506500959396405</v>
+      </c>
+      <c r="C51" s="10">
+        <v>0.163576564412375</v>
+      </c>
+      <c r="D51" s="10">
+        <v>0.13481863339742001</v>
+      </c>
+      <c r="E51" s="10">
+        <v>1.73915493640418E-3</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G51" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H51" s="10">
+        <v>1</v>
+      </c>
+      <c r="I51" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J51" s="10" t="s">
+        <v>63</v>
+      </c>
+      <c r="K51" s="10">
+        <v>0.87759036570541105</v>
+      </c>
+      <c r="L51" s="10">
+        <v>0.87840603275181495</v>
+      </c>
+      <c r="M51" s="10">
+        <v>0.90687510757939305</v>
+      </c>
+      <c r="N51" s="10">
+        <v>0.88762383534554001</v>
+      </c>
+      <c r="O51" s="10">
+        <v>1.3616777400180399E-2</v>
+      </c>
+      <c r="P51" s="10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="52" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A52" s="9">
+        <v>8</v>
+      </c>
+      <c r="B52" s="10">
+        <v>73.504405657450405</v>
+      </c>
+      <c r="C52" s="10">
+        <v>0.18930571230828</v>
+      </c>
+      <c r="D52" s="10">
+        <v>0.13464403152465801</v>
+      </c>
+      <c r="E52" s="10">
+        <v>1.95043103778005E-3</v>
+      </c>
+      <c r="F52" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="G52" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H52" s="10">
+        <v>1</v>
+      </c>
+      <c r="I52" s="10">
+        <v>1</v>
+      </c>
+      <c r="J52" s="10" t="s">
+        <v>64</v>
+      </c>
+      <c r="K52" s="10">
+        <v>0.87759036570541105</v>
+      </c>
+      <c r="L52" s="10">
+        <v>0.87840603275181495</v>
+      </c>
+      <c r="M52" s="10">
+        <v>0.90687510757939305</v>
+      </c>
+      <c r="N52" s="10">
+        <v>0.88762383534554001</v>
+      </c>
+      <c r="O52" s="10">
+        <v>1.3616777400180399E-2</v>
+      </c>
+      <c r="P52" s="10">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="53" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A53" s="9">
+        <v>33</v>
+      </c>
+      <c r="B53" s="10">
+        <v>4.4742918809254997</v>
+      </c>
+      <c r="C53" s="10">
+        <v>7.6394126184309602E-2</v>
+      </c>
+      <c r="D53" s="10">
+        <v>0.143282334009806</v>
+      </c>
+      <c r="E53" s="10">
+        <v>3.3973583089502201E-3</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G53" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H53" s="10">
+        <v>1</v>
+      </c>
+      <c r="I53" s="10">
+        <v>0.1</v>
+      </c>
+      <c r="J53" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="K53" s="10">
+        <v>0.88944107397877303</v>
+      </c>
+      <c r="L53" s="10">
+        <v>0.88889067235313401</v>
+      </c>
+      <c r="M53" s="10">
+        <v>0.88433603404769101</v>
+      </c>
+      <c r="N53" s="10">
+        <v>0.88755592679319895</v>
+      </c>
+      <c r="O53" s="10">
+        <v>2.2878690896130801E-3</v>
+      </c>
+      <c r="P53" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A54" s="9">
+        <v>34</v>
+      </c>
+      <c r="B54" s="10">
+        <v>4.4207158883412703</v>
+      </c>
+      <c r="C54" s="10">
+        <v>4.8448802726961098E-3</v>
+      </c>
+      <c r="D54" s="10">
+        <v>0.146917661031087</v>
+      </c>
+      <c r="E54" s="10">
+        <v>6.0394734750361303E-3</v>
+      </c>
+      <c r="F54" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G54" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H54" s="10">
+        <v>1</v>
+      </c>
+      <c r="I54" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="J54" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="K54" s="10">
+        <v>0.88944107397877303</v>
+      </c>
+      <c r="L54" s="10">
+        <v>0.88889067235313401</v>
+      </c>
+      <c r="M54" s="10">
+        <v>0.88433603404769101</v>
+      </c>
+      <c r="N54" s="10">
+        <v>0.88755592679319895</v>
+      </c>
+      <c r="O54" s="10">
+        <v>2.2878690896130801E-3</v>
+      </c>
+      <c r="P54" s="10">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A55" s="9">
+        <v>35</v>
+      </c>
+      <c r="B55" s="10">
+        <v>4.63816992441813</v>
+      </c>
+      <c r="C55" s="10">
+        <v>6.0931008539592199E-2</v>
+      </c>
+      <c r="D55" s="10">
+        <v>0.14264639218648301</v>
+      </c>
+      <c r="E55" s="10">
+        <v>5.9540907329544198E-3</v>
+      </c>
+      <c r="F55" s="10" t="s">
+        <v>85</v>
+      </c>
+      <c r="G55" s="10" t="s">
+        <v>55</v>
+      </c>
+      <c r="H55" s="10">
+        <v>1</v>
+      </c>
+      <c r="I55" s="10">
+        <v>1</v>
+      </c>
+      <c r="J55" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K55" s="10">
+        <v>0.88944107397877303</v>
+      </c>
+      <c r="L55" s="10">
+        <v>0.88889067235313401</v>
+      </c>
+      <c r="M55" s="10">
+        <v>0.88433603404769101</v>
+      </c>
+      <c r="N55" s="10">
+        <v>0.88755592679319895</v>
+      </c>
+      <c r="O55" s="10">
+        <v>2.2878690896130801E-3</v>
+      </c>
+      <c r="P55" s="10">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:S1" xr:uid="{EA095D1F-06E7-704F-9D76-809F97650650}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:S55">
+      <sortCondition ref="P1:P55"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final result for multi
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ajaamour/Projects/Seal-Pup-Aerial-Imagery-Classifier/results/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D6116AC-6605-5448-AD1F-1E7C2D9E6A8E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0C56439-7B63-B344-B5C9-41328D12A9F5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19280" activeTab="9" xr2:uid="{077603D1-627F-BB4C-8452-0B21DBAC2288}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19280" firstSheet="3" activeTab="12" xr2:uid="{077603D1-627F-BB4C-8452-0B21DBAC2288}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -23,17 +23,19 @@
     <sheet name="MLP Multi GS (poor)" sheetId="8" r:id="rId8"/>
     <sheet name="MLP Binary RS (old)" sheetId="9" r:id="rId9"/>
     <sheet name="MLP Binary RS (newPCA)" sheetId="13" r:id="rId10"/>
-    <sheet name="MLP Multi RS" sheetId="10" r:id="rId11"/>
-    <sheet name="MLP Multi GS" sheetId="12" r:id="rId12"/>
-    <sheet name="MLP Multi RS oversample" sheetId="11" r:id="rId13"/>
+    <sheet name="MLP Binary GS (newPCA" sheetId="14" r:id="rId11"/>
+    <sheet name="MLP Multi RS" sheetId="10" r:id="rId12"/>
+    <sheet name="MLP Multi GS" sheetId="12" r:id="rId13"/>
+    <sheet name="MLP Multi RS oversample" sheetId="11" r:id="rId14"/>
   </sheets>
   <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'MLP Binary GS (newPCA'!$A$1:$O$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'MLP Binary RS (newPCA)'!$A$1:$P$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">'MLP Binary RS (old)'!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'MLP Multi GS'!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'MLP Multi GS'!$A$1:$P$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'MLP Multi GS (poor)'!$A$1:$S$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'MLP Multi RS'!$A$1:$P$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">'MLP Multi RS oversample'!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">'MLP Multi RS'!$A$1:$P$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="13" hidden="1">'MLP Multi RS oversample'!$A$1:$P$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="861" uniqueCount="510">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="983" uniqueCount="568">
   <si>
     <t>Average accuracy</t>
   </si>
@@ -1583,6 +1585,180 @@
   </si>
   <si>
     <t>updated PCA used (475 instead of the one determined for multi)</t>
+  </si>
+  <si>
+    <t>(98,)</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>(98, 98)</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>(114,)</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>(114, 114)</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.0001, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.26, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98,), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (98, 98), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114,), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.001}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.03}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.04}</t>
+  </si>
+  <si>
+    <t>{'alpha': 0.96, 'hidden_layer_sizes': (114, 114), 'learning_rate_init': 0.1}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              hidden_layer_sizes=(114, 114), learning_rate='constant',</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              learning_rate_init=0.001, max_fun=15000, max_iter=200,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              momentum=0.9, n_iter_no_change=10, nesterovs_momentum=True,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">              tol=0.0001, validation_fraction=0.1, verbose=False,</t>
+  </si>
+  <si>
+    <t>Score: 0.992173721340388</t>
+  </si>
+  <si>
+    <t>--- Training Runtime: 7822.71 seconds ---</t>
   </si>
 </sst>
 </file>
@@ -4437,7 +4613,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B93D5527-DC76-F243-8E9D-A2C8510232DA}">
   <dimension ref="A1:S101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="C4" workbookViewId="0">
       <selection activeCell="S19" sqref="S19"/>
     </sheetView>
   </sheetViews>
@@ -9560,6 +9736,2381 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C03F6B6-FFDB-5146-B165-48925814BE41}">
+  <dimension ref="A1:R49"/>
+  <sheetViews>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="Q21" sqref="Q21"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="3.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="7.5" customWidth="1"/>
+    <col min="10" max="13" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="16.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A1" s="7"/>
+      <c r="B1" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D1" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="E1" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="F1" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="G1" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="I1" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="K1" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L1" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M1" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="N1" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A2" s="8">
+        <v>12</v>
+      </c>
+      <c r="B2" s="9">
+        <v>40.7197994391123</v>
+      </c>
+      <c r="C2" s="9">
+        <v>3.8149384499168399</v>
+      </c>
+      <c r="D2" s="9">
+        <v>0.22018583615620901</v>
+      </c>
+      <c r="E2" s="9">
+        <v>3.2072316474027001E-3</v>
+      </c>
+      <c r="F2" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H2" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I2" s="9" t="s">
+        <v>526</v>
+      </c>
+      <c r="J2" s="9">
+        <v>0.99024470899470896</v>
+      </c>
+      <c r="K2" s="9">
+        <v>0.99346891534391502</v>
+      </c>
+      <c r="L2" s="9">
+        <v>0.99280753968253999</v>
+      </c>
+      <c r="M2" s="9">
+        <v>0.99217372134038795</v>
+      </c>
+      <c r="N2" s="9">
+        <v>1.39048454712776E-3</v>
+      </c>
+      <c r="O2" s="9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A3" s="8">
+        <v>8</v>
+      </c>
+      <c r="B3" s="9">
+        <v>19.615515629450499</v>
+      </c>
+      <c r="C3" s="9">
+        <v>1.0044174451808501</v>
+      </c>
+      <c r="D3" s="9">
+        <v>0.122306903203328</v>
+      </c>
+      <c r="E3" s="9">
+        <v>4.6170366241745702E-3</v>
+      </c>
+      <c r="F3" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G3" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H3" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>521</v>
+      </c>
+      <c r="J3" s="9">
+        <v>0.99071318342151704</v>
+      </c>
+      <c r="K3" s="9">
+        <v>0.99300044091710804</v>
+      </c>
+      <c r="L3" s="9">
+        <v>0.99264219576719603</v>
+      </c>
+      <c r="M3" s="9">
+        <v>0.99211860670193996</v>
+      </c>
+      <c r="N3" s="9">
+        <v>1.0044885414066001E-3</v>
+      </c>
+      <c r="O3" s="9">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A4" s="8">
+        <v>0</v>
+      </c>
+      <c r="B4" s="9">
+        <v>18.232419729232799</v>
+      </c>
+      <c r="C4" s="9">
+        <v>4.4980446078886001</v>
+      </c>
+      <c r="D4" s="9">
+        <v>0.115511496861776</v>
+      </c>
+      <c r="E4" s="9">
+        <v>5.0019600228224598E-3</v>
+      </c>
+      <c r="F4" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G4" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H4" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I4" s="9" t="s">
+        <v>511</v>
+      </c>
+      <c r="J4" s="9">
+        <v>0.99118165784832502</v>
+      </c>
+      <c r="K4" s="9">
+        <v>0.99247685185185197</v>
+      </c>
+      <c r="L4" s="9">
+        <v>0.99247685185185197</v>
+      </c>
+      <c r="M4" s="9">
+        <v>0.99204512051734295</v>
+      </c>
+      <c r="N4" s="9">
+        <v>6.1056030856425196E-4</v>
+      </c>
+      <c r="O4" s="9">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A5" s="8">
+        <v>4</v>
+      </c>
+      <c r="B5" s="9">
+        <v>27.025415658950799</v>
+      </c>
+      <c r="C5" s="9">
+        <v>5.7784036473293501</v>
+      </c>
+      <c r="D5" s="9">
+        <v>0.17855103810628301</v>
+      </c>
+      <c r="E5" s="9">
+        <v>1.20655866043514E-2</v>
+      </c>
+      <c r="F5" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H5" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I5" s="9" t="s">
+        <v>516</v>
+      </c>
+      <c r="J5" s="9">
+        <v>0.99038249559082903</v>
+      </c>
+      <c r="K5" s="9">
+        <v>0.991236772486772</v>
+      </c>
+      <c r="L5" s="9">
+        <v>0.99184303350970004</v>
+      </c>
+      <c r="M5" s="9">
+        <v>0.99115410052910102</v>
+      </c>
+      <c r="N5" s="9">
+        <v>5.9912087959730197E-4</v>
+      </c>
+      <c r="O5" s="9">
+        <v>4</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A6" s="8">
+        <v>3</v>
+      </c>
+      <c r="B6" s="9">
+        <v>165.499751170476</v>
+      </c>
+      <c r="C6" s="9">
+        <v>3.3014095552268499</v>
+      </c>
+      <c r="D6" s="9">
+        <v>0.22939332326253301</v>
+      </c>
+      <c r="E6" s="9">
+        <v>9.8556916314673504E-2</v>
+      </c>
+      <c r="F6" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H6" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I6" s="9" t="s">
+        <v>514</v>
+      </c>
+      <c r="J6" s="9">
+        <v>0.98768187830687804</v>
+      </c>
+      <c r="K6" s="9">
+        <v>0.99209104938271597</v>
+      </c>
+      <c r="L6" s="9">
+        <v>0.99038249559082903</v>
+      </c>
+      <c r="M6" s="9">
+        <v>0.99005180776014101</v>
+      </c>
+      <c r="N6" s="9">
+        <v>1.8151608239170801E-3</v>
+      </c>
+      <c r="O6" s="9">
+        <v>5</v>
+      </c>
+      <c r="Q6" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A7" s="8">
+        <v>11</v>
+      </c>
+      <c r="B7" s="9">
+        <v>174.260065396627</v>
+      </c>
+      <c r="C7" s="9">
+        <v>8.5627287759760708</v>
+      </c>
+      <c r="D7" s="9">
+        <v>0.273455619812012</v>
+      </c>
+      <c r="E7" s="9">
+        <v>0.104745698852286</v>
+      </c>
+      <c r="F7" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G7" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H7" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I7" s="9" t="s">
+        <v>524</v>
+      </c>
+      <c r="J7" s="9">
+        <v>0.98817791005291</v>
+      </c>
+      <c r="K7" s="9">
+        <v>0.99214616402116396</v>
+      </c>
+      <c r="L7" s="9">
+        <v>0.988949514991182</v>
+      </c>
+      <c r="M7" s="9">
+        <v>0.98975786302175195</v>
+      </c>
+      <c r="N7" s="9">
+        <v>1.7179114825927699E-3</v>
+      </c>
+      <c r="O7" s="9">
+        <v>6</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A8" s="8">
+        <v>10</v>
+      </c>
+      <c r="B8" s="9">
+        <v>163.89012869199101</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1.3945600515079399</v>
+      </c>
+      <c r="D8" s="9">
+        <v>0.13283507029215499</v>
+      </c>
+      <c r="E8" s="9">
+        <v>2.0238129917504101E-2</v>
+      </c>
+      <c r="F8" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G8" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H8" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I8" s="9" t="s">
+        <v>523</v>
+      </c>
+      <c r="J8" s="9">
+        <v>0.98699294532627901</v>
+      </c>
+      <c r="K8" s="9">
+        <v>0.99063051146384495</v>
+      </c>
+      <c r="L8" s="9">
+        <v>0.99159501763668401</v>
+      </c>
+      <c r="M8" s="9">
+        <v>0.98973949147560303</v>
+      </c>
+      <c r="N8" s="9">
+        <v>1.9816163187553102E-3</v>
+      </c>
+      <c r="O8" s="9">
+        <v>7</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A9" s="8">
+        <v>24</v>
+      </c>
+      <c r="B9" s="9">
+        <v>91.705610354741395</v>
+      </c>
+      <c r="C9" s="9">
+        <v>20.265205019526999</v>
+      </c>
+      <c r="D9" s="9">
+        <v>0.35771131515502902</v>
+      </c>
+      <c r="E9" s="9">
+        <v>7.3284660394083698E-2</v>
+      </c>
+      <c r="F9" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G9" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H9" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I9" s="9" t="s">
+        <v>538</v>
+      </c>
+      <c r="J9" s="9">
+        <v>0.98531194885361595</v>
+      </c>
+      <c r="K9" s="9">
+        <v>0.99198082010582</v>
+      </c>
+      <c r="L9" s="9">
+        <v>0.99087852733686099</v>
+      </c>
+      <c r="M9" s="9">
+        <v>0.98939043209876498</v>
+      </c>
+      <c r="N9" s="9">
+        <v>2.9188218539736798E-3</v>
+      </c>
+      <c r="O9" s="9">
+        <v>8</v>
+      </c>
+      <c r="Q9" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A10" s="8">
+        <v>16</v>
+      </c>
+      <c r="B10" s="9">
+        <v>73.181618531544999</v>
+      </c>
+      <c r="C10" s="9">
+        <v>22.3282648898109</v>
+      </c>
+      <c r="D10" s="9">
+        <v>0.37937132517496702</v>
+      </c>
+      <c r="E10" s="9">
+        <v>0.196193648729274</v>
+      </c>
+      <c r="F10" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H10" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I10" s="9" t="s">
+        <v>530</v>
+      </c>
+      <c r="J10" s="9">
+        <v>0.98533950617284005</v>
+      </c>
+      <c r="K10" s="9">
+        <v>0.99151234567901203</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0.99112654320987703</v>
+      </c>
+      <c r="M10" s="9">
+        <v>0.98932613168724304</v>
+      </c>
+      <c r="N10" s="9">
+        <v>2.8233665637989098E-3</v>
+      </c>
+      <c r="O10" s="9">
+        <v>9</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>564</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A11" s="8">
+        <v>2</v>
+      </c>
+      <c r="B11" s="9">
+        <v>116.914597988129</v>
+      </c>
+      <c r="C11" s="9">
+        <v>74.7467277021494</v>
+      </c>
+      <c r="D11" s="9">
+        <v>0.12937474250793499</v>
+      </c>
+      <c r="E11" s="9">
+        <v>8.2015244416784698E-3</v>
+      </c>
+      <c r="F11" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G11" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H11" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I11" s="9" t="s">
+        <v>513</v>
+      </c>
+      <c r="J11" s="9">
+        <v>0.98128858024691401</v>
+      </c>
+      <c r="K11" s="9">
+        <v>0.990465167548501</v>
+      </c>
+      <c r="L11" s="9">
+        <v>0.99071318342151704</v>
+      </c>
+      <c r="M11" s="9">
+        <v>0.98748897707230998</v>
+      </c>
+      <c r="N11" s="9">
+        <v>4.38551164347713E-3</v>
+      </c>
+      <c r="O11" s="9">
+        <v>10</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A12" s="8">
+        <v>36</v>
+      </c>
+      <c r="B12" s="9">
+        <v>102.373891750971</v>
+      </c>
+      <c r="C12" s="9">
+        <v>6.9333849983746099</v>
+      </c>
+      <c r="D12" s="9">
+        <v>1.06069731712341</v>
+      </c>
+      <c r="E12" s="9">
+        <v>0.39611405469182398</v>
+      </c>
+      <c r="F12" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G12" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H12" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I12" s="9" t="s">
+        <v>550</v>
+      </c>
+      <c r="J12" s="9">
+        <v>0.98057208994709</v>
+      </c>
+      <c r="K12" s="9">
+        <v>0.99043761022927701</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0.98823302469135799</v>
+      </c>
+      <c r="M12" s="9">
+        <v>0.98641424162257496</v>
+      </c>
+      <c r="N12" s="9">
+        <v>4.22793105415475E-3</v>
+      </c>
+      <c r="O12" s="9">
+        <v>11</v>
+      </c>
+      <c r="Q12" t="s">
+        <v>565</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A13" s="8">
+        <v>28</v>
+      </c>
+      <c r="B13" s="9">
+        <v>69.604177157084195</v>
+      </c>
+      <c r="C13" s="9">
+        <v>20.333437348211302</v>
+      </c>
+      <c r="D13" s="9">
+        <v>0.61008461316426599</v>
+      </c>
+      <c r="E13" s="9">
+        <v>0.56656027703547196</v>
+      </c>
+      <c r="F13" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G13" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H13" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I13" s="9" t="s">
+        <v>542</v>
+      </c>
+      <c r="J13" s="9">
+        <v>0.97610780423280397</v>
+      </c>
+      <c r="K13" s="9">
+        <v>0.98936287477954099</v>
+      </c>
+      <c r="L13" s="9">
+        <v>0.99068562610229305</v>
+      </c>
+      <c r="M13" s="9">
+        <v>0.98538543503821296</v>
+      </c>
+      <c r="N13" s="9">
+        <v>6.5824637123476299E-3</v>
+      </c>
+      <c r="O13" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A14" s="8">
+        <v>44</v>
+      </c>
+      <c r="B14" s="9">
+        <v>126.472374677658</v>
+      </c>
+      <c r="C14" s="9">
+        <v>24.8921918239107</v>
+      </c>
+      <c r="D14" s="9">
+        <v>1.32500696182251</v>
+      </c>
+      <c r="E14" s="9">
+        <v>0.121684818499459</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G14" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H14" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I14" s="9" t="s">
+        <v>558</v>
+      </c>
+      <c r="J14" s="9">
+        <v>0.98250110229276899</v>
+      </c>
+      <c r="K14" s="9">
+        <v>0.98848104056437402</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0.98517416225749599</v>
+      </c>
+      <c r="M14" s="9">
+        <v>0.98538543503821296</v>
+      </c>
+      <c r="N14" s="9">
+        <v>2.4458662506298698E-3</v>
+      </c>
+      <c r="O14" s="9">
+        <v>12</v>
+      </c>
+      <c r="Q14" t="s">
+        <v>566</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A15" s="8">
+        <v>32</v>
+      </c>
+      <c r="B15" s="9">
+        <v>85.869278430938706</v>
+      </c>
+      <c r="C15" s="9">
+        <v>20.067440121119901</v>
+      </c>
+      <c r="D15" s="9">
+        <v>0.192653020222982</v>
+      </c>
+      <c r="E15" s="9">
+        <v>2.35822033939477E-2</v>
+      </c>
+      <c r="F15" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G15" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H15" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I15" s="9" t="s">
+        <v>546</v>
+      </c>
+      <c r="J15" s="9">
+        <v>0.980930335097002</v>
+      </c>
+      <c r="K15" s="9">
+        <v>0.987433862433862</v>
+      </c>
+      <c r="L15" s="9">
+        <v>0.98644179894179895</v>
+      </c>
+      <c r="M15" s="9">
+        <v>0.98493533215755502</v>
+      </c>
+      <c r="N15" s="9">
+        <v>2.8607747883335798E-3</v>
+      </c>
+      <c r="O15" s="9">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A16" s="8">
+        <v>40</v>
+      </c>
+      <c r="B16" s="9">
+        <v>103.91432539621999</v>
+      </c>
+      <c r="C16" s="9">
+        <v>13.123215319713699</v>
+      </c>
+      <c r="D16" s="9">
+        <v>0.48166433970133499</v>
+      </c>
+      <c r="E16" s="9">
+        <v>7.4654497095115097E-2</v>
+      </c>
+      <c r="F16" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G16" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H16" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I16" s="9" t="s">
+        <v>554</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0.97985559964726598</v>
+      </c>
+      <c r="K16" s="9">
+        <v>0.98713073192239897</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0.98746141975308599</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0.98481591710758398</v>
+      </c>
+      <c r="N16" s="9">
+        <v>3.5100712804432802E-3</v>
+      </c>
+      <c r="O16" s="9">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A17" s="8">
+        <v>1</v>
+      </c>
+      <c r="B17" s="9">
+        <v>12.5824445883433</v>
+      </c>
+      <c r="C17" s="9">
+        <v>2.0464968893040298</v>
+      </c>
+      <c r="D17" s="9">
+        <v>0.11529342333475701</v>
+      </c>
+      <c r="E17" s="9">
+        <v>7.2525207487678803E-3</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G17" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I17" s="9" t="s">
+        <v>512</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0.98194995590828904</v>
+      </c>
+      <c r="K17" s="9">
+        <v>0.985532407407407</v>
+      </c>
+      <c r="L17" s="9">
+        <v>0.98638668430335097</v>
+      </c>
+      <c r="M17" s="9">
+        <v>0.98462301587301604</v>
+      </c>
+      <c r="N17" s="9">
+        <v>1.9220448199775799E-3</v>
+      </c>
+      <c r="O17" s="9">
+        <v>16</v>
+      </c>
+      <c r="Q17" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A18" s="8">
+        <v>20</v>
+      </c>
+      <c r="B18" s="9">
+        <v>93.3942433198293</v>
+      </c>
+      <c r="C18" s="9">
+        <v>42.177726277090002</v>
+      </c>
+      <c r="D18" s="9">
+        <v>0.83331569035847997</v>
+      </c>
+      <c r="E18" s="9">
+        <v>0.49962727342331897</v>
+      </c>
+      <c r="F18" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G18" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H18" s="9">
+        <v>1E-3</v>
+      </c>
+      <c r="I18" s="9" t="s">
+        <v>534</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0.977127425044092</v>
+      </c>
+      <c r="K18" s="9">
+        <v>0.98790233686066997</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0.98787477954144598</v>
+      </c>
+      <c r="M18" s="9">
+        <v>0.98430151381540298</v>
+      </c>
+      <c r="N18" s="9">
+        <v>5.0728592940240203E-3</v>
+      </c>
+      <c r="O18" s="9">
+        <v>17</v>
+      </c>
+      <c r="Q18">
+        <f>7822/60</f>
+        <v>130.36666666666667</v>
+      </c>
+      <c r="R18" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A19" s="8">
+        <v>9</v>
+      </c>
+      <c r="B19" s="9">
+        <v>9.8533626397450806</v>
+      </c>
+      <c r="C19" s="9">
+        <v>0.19309926643393199</v>
+      </c>
+      <c r="D19" s="9">
+        <v>0.12006497383117699</v>
+      </c>
+      <c r="E19" s="9">
+        <v>1.03623507666586E-3</v>
+      </c>
+      <c r="F19" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G19" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H19" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I19" s="9" t="s">
+        <v>522</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0.98139880952380998</v>
+      </c>
+      <c r="K19" s="9">
+        <v>0.98465057319224003</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0.98547729276896001</v>
+      </c>
+      <c r="M19" s="9">
+        <v>0.98384222516166997</v>
+      </c>
+      <c r="N19" s="9">
+        <v>1.7604121296138199E-3</v>
+      </c>
+      <c r="O19" s="9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A20" s="8">
+        <v>17</v>
+      </c>
+      <c r="B20" s="9">
+        <v>33.207441647847503</v>
+      </c>
+      <c r="C20" s="9">
+        <v>6.6026830129669598</v>
+      </c>
+      <c r="D20" s="9">
+        <v>0.14478397369384799</v>
+      </c>
+      <c r="E20" s="9">
+        <v>5.7530766755844197E-2</v>
+      </c>
+      <c r="F20" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H20" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I20" s="9" t="s">
+        <v>531</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0.95714836860670205</v>
+      </c>
+      <c r="K20" s="9">
+        <v>0.95888447971781299</v>
+      </c>
+      <c r="L20" s="9">
+        <v>0.95863646384479695</v>
+      </c>
+      <c r="M20" s="9">
+        <v>0.95822310405643696</v>
+      </c>
+      <c r="N20" s="9">
+        <v>7.6666819572551801E-4</v>
+      </c>
+      <c r="O20" s="9">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A21" s="8">
+        <v>25</v>
+      </c>
+      <c r="B21" s="9">
+        <v>41.526197274525998</v>
+      </c>
+      <c r="C21" s="9">
+        <v>23.534408972722101</v>
+      </c>
+      <c r="D21" s="9">
+        <v>0.11671503384908</v>
+      </c>
+      <c r="E21" s="9">
+        <v>1.70214829842006E-2</v>
+      </c>
+      <c r="F21" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H21" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I21" s="9" t="s">
+        <v>539</v>
+      </c>
+      <c r="J21" s="9">
+        <v>0.95403439153439196</v>
+      </c>
+      <c r="K21" s="9">
+        <v>0.96073082010582</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0.95681768077601403</v>
+      </c>
+      <c r="M21" s="9">
+        <v>0.95719429747207496</v>
+      </c>
+      <c r="N21" s="9">
+        <v>2.74674583278411E-3</v>
+      </c>
+      <c r="O21" s="9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A22" s="8">
+        <v>29</v>
+      </c>
+      <c r="B22" s="9">
+        <v>50.890259424845397</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2.8820349462424502</v>
+      </c>
+      <c r="D22" s="9">
+        <v>0.24601085980733201</v>
+      </c>
+      <c r="E22" s="9">
+        <v>1.5345644176191799E-2</v>
+      </c>
+      <c r="F22" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G22" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H22" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I22" s="9" t="s">
+        <v>543</v>
+      </c>
+      <c r="J22" s="9">
+        <v>0.95271164021164001</v>
+      </c>
+      <c r="K22" s="9">
+        <v>0.95505401234567899</v>
+      </c>
+      <c r="L22" s="9">
+        <v>0.95852623456790098</v>
+      </c>
+      <c r="M22" s="9">
+        <v>0.95543062904174003</v>
+      </c>
+      <c r="N22" s="9">
+        <v>2.3886895966588701E-3</v>
+      </c>
+      <c r="O22" s="9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A23" s="8">
+        <v>21</v>
+      </c>
+      <c r="B23" s="9">
+        <v>50.432075421015398</v>
+      </c>
+      <c r="C23" s="9">
+        <v>12.6105618724756</v>
+      </c>
+      <c r="D23" s="9">
+        <v>0.26419115066528298</v>
+      </c>
+      <c r="E23" s="9">
+        <v>5.8350459250668299E-2</v>
+      </c>
+      <c r="F23" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G23" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H23" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I23" s="9" t="s">
+        <v>535</v>
+      </c>
+      <c r="J23" s="9">
+        <v>0.95323522927689597</v>
+      </c>
+      <c r="K23" s="9">
+        <v>0.95483355379188695</v>
+      </c>
+      <c r="L23" s="9">
+        <v>0.95756172839506204</v>
+      </c>
+      <c r="M23" s="9">
+        <v>0.95521017048794798</v>
+      </c>
+      <c r="N23" s="9">
+        <v>1.7862490973519899E-3</v>
+      </c>
+      <c r="O23" s="9">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A24" s="8">
+        <v>22</v>
+      </c>
+      <c r="B24" s="9">
+        <v>39.192319552103697</v>
+      </c>
+      <c r="C24" s="9">
+        <v>4.3229433433226498</v>
+      </c>
+      <c r="D24" s="9">
+        <v>0.19171524047851601</v>
+      </c>
+      <c r="E24" s="9">
+        <v>1.19569147408666E-2</v>
+      </c>
+      <c r="F24" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G24" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H24" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I24" s="9" t="s">
+        <v>536</v>
+      </c>
+      <c r="J24" s="9">
+        <v>0.95152667548500902</v>
+      </c>
+      <c r="K24" s="9">
+        <v>0.95081018518518501</v>
+      </c>
+      <c r="L24" s="9">
+        <v>0.95499889770723101</v>
+      </c>
+      <c r="M24" s="9">
+        <v>0.95244525279247505</v>
+      </c>
+      <c r="N24" s="9">
+        <v>1.8292377921654899E-3</v>
+      </c>
+      <c r="O24" s="9">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A25" s="8">
+        <v>30</v>
+      </c>
+      <c r="B25" s="9">
+        <v>46.449179967244497</v>
+      </c>
+      <c r="C25" s="9">
+        <v>4.94384444536872</v>
+      </c>
+      <c r="D25" s="9">
+        <v>0.191287358601888</v>
+      </c>
+      <c r="E25" s="9">
+        <v>4.7992453626036101E-3</v>
+      </c>
+      <c r="F25" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G25" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H25" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I25" s="9" t="s">
+        <v>544</v>
+      </c>
+      <c r="J25" s="9">
+        <v>0.94810956790123502</v>
+      </c>
+      <c r="K25" s="9">
+        <v>0.95364858906525596</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0.95510912698412698</v>
+      </c>
+      <c r="M25" s="9">
+        <v>0.95228909465020595</v>
+      </c>
+      <c r="N25" s="9">
+        <v>3.0149212966111799E-3</v>
+      </c>
+      <c r="O25" s="9">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A26" s="8">
+        <v>18</v>
+      </c>
+      <c r="B26" s="9">
+        <v>28.892050027847301</v>
+      </c>
+      <c r="C26" s="9">
+        <v>4.7080896410448201</v>
+      </c>
+      <c r="D26" s="9">
+        <v>0.156785647074382</v>
+      </c>
+      <c r="E26" s="9">
+        <v>6.8346042082738298E-2</v>
+      </c>
+      <c r="F26" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G26" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H26" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I26" s="9" t="s">
+        <v>532</v>
+      </c>
+      <c r="J26" s="9">
+        <v>0.94844025573192203</v>
+      </c>
+      <c r="K26" s="9">
+        <v>0.95287698412698396</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0.95444775132275095</v>
+      </c>
+      <c r="M26" s="9">
+        <v>0.95192166372721898</v>
+      </c>
+      <c r="N26" s="9">
+        <v>2.54387874686306E-3</v>
+      </c>
+      <c r="O26" s="9">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A27" s="8">
+        <v>45</v>
+      </c>
+      <c r="B27" s="9">
+        <v>37.572816610336297</v>
+      </c>
+      <c r="C27" s="9">
+        <v>4.2902545264022001</v>
+      </c>
+      <c r="D27" s="9">
+        <v>0.215855280558268</v>
+      </c>
+      <c r="E27" s="9">
+        <v>2.0625362899439999E-2</v>
+      </c>
+      <c r="F27" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G27" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H27" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I27" s="9" t="s">
+        <v>559</v>
+      </c>
+      <c r="J27" s="9">
+        <v>0.94888117283950602</v>
+      </c>
+      <c r="K27" s="9">
+        <v>0.95229828042328102</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0.95061728395061695</v>
+      </c>
+      <c r="M27" s="9">
+        <v>0.95059891240446803</v>
+      </c>
+      <c r="N27" s="9">
+        <v>1.39508881319505E-3</v>
+      </c>
+      <c r="O27" s="9">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A28" s="8">
+        <v>26</v>
+      </c>
+      <c r="B28" s="9">
+        <v>53.722900867462201</v>
+      </c>
+      <c r="C28" s="9">
+        <v>16.1707195234879</v>
+      </c>
+      <c r="D28" s="9">
+        <v>0.20580299695332799</v>
+      </c>
+      <c r="E28" s="9">
+        <v>0.112585180835306</v>
+      </c>
+      <c r="F28" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G28" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H28" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I28" s="9" t="s">
+        <v>540</v>
+      </c>
+      <c r="J28" s="9">
+        <v>0.94675925925925897</v>
+      </c>
+      <c r="K28" s="9">
+        <v>0.95318011463844798</v>
+      </c>
+      <c r="L28" s="9">
+        <v>0.95023148148148195</v>
+      </c>
+      <c r="M28" s="9">
+        <v>0.95005695179306304</v>
+      </c>
+      <c r="N28" s="9">
+        <v>2.6242067257514498E-3</v>
+      </c>
+      <c r="O28" s="9">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A29" s="8">
+        <v>37</v>
+      </c>
+      <c r="B29" s="9">
+        <v>34.544801314671801</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2.3710705150951599</v>
+      </c>
+      <c r="D29" s="9">
+        <v>0.18268505732218401</v>
+      </c>
+      <c r="E29" s="9">
+        <v>3.0135743495922299E-3</v>
+      </c>
+      <c r="F29" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H29" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I29" s="9" t="s">
+        <v>551</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0.94502314814814803</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0.94868827160493796</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0.95513668430335097</v>
+      </c>
+      <c r="M29" s="9">
+        <v>0.94961603468547895</v>
+      </c>
+      <c r="N29" s="9">
+        <v>4.1806268781017101E-3</v>
+      </c>
+      <c r="O29" s="9">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A30" s="8">
+        <v>33</v>
+      </c>
+      <c r="B30" s="9">
+        <v>31.8077755769094</v>
+      </c>
+      <c r="C30" s="9">
+        <v>8.5197856042358708</v>
+      </c>
+      <c r="D30" s="9">
+        <v>0.11127424240112301</v>
+      </c>
+      <c r="E30" s="9">
+        <v>2.37090042786343E-3</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H30" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I30" s="9" t="s">
+        <v>547</v>
+      </c>
+      <c r="J30" s="9">
+        <v>0.94753086419753096</v>
+      </c>
+      <c r="K30" s="9">
+        <v>0.95318011463844798</v>
+      </c>
+      <c r="L30" s="9">
+        <v>0.94797178130511495</v>
+      </c>
+      <c r="M30" s="9">
+        <v>0.94956092004703097</v>
+      </c>
+      <c r="N30" s="9">
+        <v>2.5654796941762099E-3</v>
+      </c>
+      <c r="O30" s="9">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A31" s="8">
+        <v>41</v>
+      </c>
+      <c r="B31" s="9">
+        <v>28.269587993621801</v>
+      </c>
+      <c r="C31" s="9">
+        <v>3.5294153969557498</v>
+      </c>
+      <c r="D31" s="9">
+        <v>0.107870737711589</v>
+      </c>
+      <c r="E31" s="9">
+        <v>2.4738155696155699E-3</v>
+      </c>
+      <c r="F31" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G31" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H31" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I31" s="9" t="s">
+        <v>555</v>
+      </c>
+      <c r="J31" s="9">
+        <v>0.94535383597883604</v>
+      </c>
+      <c r="K31" s="9">
+        <v>0.95092041446208098</v>
+      </c>
+      <c r="L31" s="9">
+        <v>0.94910163139329795</v>
+      </c>
+      <c r="M31" s="9">
+        <v>0.94845862727807195</v>
+      </c>
+      <c r="N31" s="9">
+        <v>2.31758347158997E-3</v>
+      </c>
+      <c r="O31" s="9">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A32" s="8">
+        <v>42</v>
+      </c>
+      <c r="B32" s="9">
+        <v>36.731898943583197</v>
+      </c>
+      <c r="C32" s="9">
+        <v>6.9173681442497399</v>
+      </c>
+      <c r="D32" s="9">
+        <v>0.103667338689168</v>
+      </c>
+      <c r="E32" s="9">
+        <v>2.49841158711692E-4</v>
+      </c>
+      <c r="F32" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G32" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H32" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I32" s="9" t="s">
+        <v>556</v>
+      </c>
+      <c r="J32" s="9">
+        <v>0.93857473544973602</v>
+      </c>
+      <c r="K32" s="9">
+        <v>0.94827491181657897</v>
+      </c>
+      <c r="L32" s="9">
+        <v>0.94177138447971798</v>
+      </c>
+      <c r="M32" s="9">
+        <v>0.94287367724867699</v>
+      </c>
+      <c r="N32" s="9">
+        <v>4.03605768032291E-3</v>
+      </c>
+      <c r="O32" s="9">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="33" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A33" s="8">
+        <v>38</v>
+      </c>
+      <c r="B33" s="9">
+        <v>30.705408334732098</v>
+      </c>
+      <c r="C33" s="9">
+        <v>2.1884128065788402</v>
+      </c>
+      <c r="D33" s="9">
+        <v>0.1809983253479</v>
+      </c>
+      <c r="E33" s="9">
+        <v>5.0402991463858998E-3</v>
+      </c>
+      <c r="F33" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G33" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H33" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I33" s="9" t="s">
+        <v>552</v>
+      </c>
+      <c r="J33" s="9">
+        <v>0.93777557319224003</v>
+      </c>
+      <c r="K33" s="9">
+        <v>0.94491291887125195</v>
+      </c>
+      <c r="L33" s="9">
+        <v>0.94460978835978804</v>
+      </c>
+      <c r="M33" s="9">
+        <v>0.94243276014109401</v>
+      </c>
+      <c r="N33" s="9">
+        <v>3.2954529010111901E-3</v>
+      </c>
+      <c r="O33" s="9">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="34" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A34" s="8">
+        <v>46</v>
+      </c>
+      <c r="B34" s="9">
+        <v>36.8023297786713</v>
+      </c>
+      <c r="C34" s="9">
+        <v>4.9673029595813203</v>
+      </c>
+      <c r="D34" s="9">
+        <v>0.20149095853169799</v>
+      </c>
+      <c r="E34" s="9">
+        <v>6.5187564342332801E-3</v>
+      </c>
+      <c r="F34" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G34" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H34" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I34" s="9" t="s">
+        <v>560</v>
+      </c>
+      <c r="J34" s="9">
+        <v>0.93807870370370405</v>
+      </c>
+      <c r="K34" s="9">
+        <v>0.94122023809523803</v>
+      </c>
+      <c r="L34" s="9">
+        <v>0.944361772486772</v>
+      </c>
+      <c r="M34" s="9">
+        <v>0.94122023809523803</v>
+      </c>
+      <c r="N34" s="9">
+        <v>2.5650520895546701E-3</v>
+      </c>
+      <c r="O34" s="9">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A35" s="8">
+        <v>34</v>
+      </c>
+      <c r="B35" s="9">
+        <v>28.695666631062799</v>
+      </c>
+      <c r="C35" s="9">
+        <v>10.3997467846908</v>
+      </c>
+      <c r="D35" s="9">
+        <v>0.108762343724569</v>
+      </c>
+      <c r="E35" s="9">
+        <v>1.1623805546504E-3</v>
+      </c>
+      <c r="F35" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G35" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H35" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I35" s="9" t="s">
+        <v>548</v>
+      </c>
+      <c r="J35" s="9">
+        <v>0.94039351851851904</v>
+      </c>
+      <c r="K35" s="9">
+        <v>0.94747574955908298</v>
+      </c>
+      <c r="L35" s="9">
+        <v>0.93039021164021196</v>
+      </c>
+      <c r="M35" s="9">
+        <v>0.93941982657260403</v>
+      </c>
+      <c r="N35" s="9">
+        <v>7.0090398057770301E-3</v>
+      </c>
+      <c r="O35" s="9">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="36" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A36" s="8">
+        <v>19</v>
+      </c>
+      <c r="B36" s="9">
+        <v>39.766828854878703</v>
+      </c>
+      <c r="C36" s="9">
+        <v>14.260664710652801</v>
+      </c>
+      <c r="D36" s="9">
+        <v>0.124279657999674</v>
+      </c>
+      <c r="E36" s="9">
+        <v>1.1260541768601799E-2</v>
+      </c>
+      <c r="F36" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G36" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H36" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I36" s="9" t="s">
+        <v>533</v>
+      </c>
+      <c r="J36" s="9">
+        <v>0.93163029100529104</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0.93975970017636701</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0.93904320987654299</v>
+      </c>
+      <c r="M36" s="9">
+        <v>0.93681106701939998</v>
+      </c>
+      <c r="N36" s="9">
+        <v>3.6750210583263699E-3</v>
+      </c>
+      <c r="O36" s="9">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="37" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A37" s="8">
+        <v>27</v>
+      </c>
+      <c r="B37" s="9">
+        <v>40.548020680745402</v>
+      </c>
+      <c r="C37" s="9">
+        <v>1.0239416029288999</v>
+      </c>
+      <c r="D37" s="9">
+        <v>0.128307104110718</v>
+      </c>
+      <c r="E37" s="9">
+        <v>2.20255256072567E-2</v>
+      </c>
+      <c r="F37" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G37" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H37" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I37" s="9" t="s">
+        <v>541</v>
+      </c>
+      <c r="J37" s="9">
+        <v>0.92380401234567899</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0.92559523809523803</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0.93813381834215204</v>
+      </c>
+      <c r="M37" s="9">
+        <v>0.92917768959435598</v>
+      </c>
+      <c r="N37" s="9">
+        <v>6.37501916503193E-3</v>
+      </c>
+      <c r="O37" s="9">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A38" s="8">
+        <v>31</v>
+      </c>
+      <c r="B38" s="9">
+        <v>59.4791120688121</v>
+      </c>
+      <c r="C38" s="9">
+        <v>19.602677649429001</v>
+      </c>
+      <c r="D38" s="9">
+        <v>0.238084634145101</v>
+      </c>
+      <c r="E38" s="9">
+        <v>3.1916796741673502E-3</v>
+      </c>
+      <c r="F38" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G38" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H38" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I38" s="9" t="s">
+        <v>545</v>
+      </c>
+      <c r="J38" s="9">
+        <v>0.93314594356261005</v>
+      </c>
+      <c r="K38" s="9">
+        <v>0.94204695767195801</v>
+      </c>
+      <c r="L38" s="9">
+        <v>0.90842702821869503</v>
+      </c>
+      <c r="M38" s="9">
+        <v>0.92787330981775396</v>
+      </c>
+      <c r="N38" s="9">
+        <v>1.4222644247024701E-2</v>
+      </c>
+      <c r="O38" s="9">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A39" s="8">
+        <v>13</v>
+      </c>
+      <c r="B39" s="9">
+        <v>24.051945527394601</v>
+      </c>
+      <c r="C39" s="9">
+        <v>4.0834639016377201</v>
+      </c>
+      <c r="D39" s="9">
+        <v>0.209229389826457</v>
+      </c>
+      <c r="E39" s="9">
+        <v>1.01292801414288E-2</v>
+      </c>
+      <c r="F39" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G39" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H39" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I39" s="9" t="s">
+        <v>527</v>
+      </c>
+      <c r="J39" s="9">
+        <v>0.97211199294532602</v>
+      </c>
+      <c r="K39" s="9">
+        <v>0.98564263668430296</v>
+      </c>
+      <c r="L39" s="9">
+        <v>0.81475970017636701</v>
+      </c>
+      <c r="M39" s="9">
+        <v>0.92417144326866596</v>
+      </c>
+      <c r="N39" s="9">
+        <v>7.7562734715708903E-2</v>
+      </c>
+      <c r="O39" s="9">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A40" s="8">
+        <v>35</v>
+      </c>
+      <c r="B40" s="9">
+        <v>24.510599454244002</v>
+      </c>
+      <c r="C40" s="9">
+        <v>4.8394365321995698</v>
+      </c>
+      <c r="D40" s="9">
+        <v>0.11266016960144</v>
+      </c>
+      <c r="E40" s="9">
+        <v>2.6177209775006898E-3</v>
+      </c>
+      <c r="F40" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G40" s="9" t="s">
+        <v>510</v>
+      </c>
+      <c r="H40" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I40" s="9" t="s">
+        <v>549</v>
+      </c>
+      <c r="J40" s="9">
+        <v>0.91782407407407396</v>
+      </c>
+      <c r="K40" s="9">
+        <v>0.92165454144620795</v>
+      </c>
+      <c r="L40" s="9">
+        <v>0.93264991181657897</v>
+      </c>
+      <c r="M40" s="9">
+        <v>0.92404284244561996</v>
+      </c>
+      <c r="N40" s="9">
+        <v>6.2838073617625702E-3</v>
+      </c>
+      <c r="O40" s="9">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A41" s="8">
+        <v>39</v>
+      </c>
+      <c r="B41" s="9">
+        <v>31.423179626464801</v>
+      </c>
+      <c r="C41" s="9">
+        <v>2.3055485163704299</v>
+      </c>
+      <c r="D41" s="9">
+        <v>0.177677392959595</v>
+      </c>
+      <c r="E41" s="9">
+        <v>4.5155828366197897E-3</v>
+      </c>
+      <c r="F41" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G41" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H41" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I41" s="9" t="s">
+        <v>553</v>
+      </c>
+      <c r="J41" s="9">
+        <v>0.92115850970017599</v>
+      </c>
+      <c r="K41" s="9">
+        <v>0.91961529982363299</v>
+      </c>
+      <c r="L41" s="9">
+        <v>0.92115850970017599</v>
+      </c>
+      <c r="M41" s="9">
+        <v>0.92064410640799499</v>
+      </c>
+      <c r="N41" s="9">
+        <v>7.2747611233184197E-4</v>
+      </c>
+      <c r="O41" s="9">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A42" s="8">
+        <v>43</v>
+      </c>
+      <c r="B42" s="9">
+        <v>32.937315066655501</v>
+      </c>
+      <c r="C42" s="9">
+        <v>9.0739194533304399</v>
+      </c>
+      <c r="D42" s="9">
+        <v>0.107180674870809</v>
+      </c>
+      <c r="E42" s="9">
+        <v>6.6121173506289198E-3</v>
+      </c>
+      <c r="F42" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G42" s="9" t="s">
+        <v>520</v>
+      </c>
+      <c r="H42" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I42" s="9" t="s">
+        <v>557</v>
+      </c>
+      <c r="J42" s="9">
+        <v>0.92000110229276899</v>
+      </c>
+      <c r="K42" s="9">
+        <v>0.91385582010582</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0.92333553791887102</v>
+      </c>
+      <c r="M42" s="9">
+        <v>0.91906415343915404</v>
+      </c>
+      <c r="N42" s="9">
+        <v>3.9263780866924799E-3</v>
+      </c>
+      <c r="O42" s="9">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A43" s="8">
+        <v>47</v>
+      </c>
+      <c r="B43" s="9">
+        <v>35.755493720372499</v>
+      </c>
+      <c r="C43" s="9">
+        <v>6.8630810197593197</v>
+      </c>
+      <c r="D43" s="9">
+        <v>0.212575674057007</v>
+      </c>
+      <c r="E43" s="9">
+        <v>1.6314114029204699E-2</v>
+      </c>
+      <c r="F43" s="9">
+        <v>0.96</v>
+      </c>
+      <c r="G43" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H43" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I43" s="9" t="s">
+        <v>561</v>
+      </c>
+      <c r="J43" s="9">
+        <v>0.91625330687830697</v>
+      </c>
+      <c r="K43" s="9">
+        <v>0.91399360670193996</v>
+      </c>
+      <c r="L43" s="9">
+        <v>0.91410383597883604</v>
+      </c>
+      <c r="M43" s="9">
+        <v>0.91478358318636099</v>
+      </c>
+      <c r="N43" s="9">
+        <v>1.04022543113551E-3</v>
+      </c>
+      <c r="O43" s="9">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A44" s="8">
+        <v>23</v>
+      </c>
+      <c r="B44" s="9">
+        <v>33.357439041137702</v>
+      </c>
+      <c r="C44" s="9">
+        <v>6.7272698725801199</v>
+      </c>
+      <c r="D44" s="9">
+        <v>0.176160971323649</v>
+      </c>
+      <c r="E44" s="9">
+        <v>5.6706700826519704E-3</v>
+      </c>
+      <c r="F44" s="9">
+        <v>0.26</v>
+      </c>
+      <c r="G44" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H44" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I44" s="9" t="s">
+        <v>537</v>
+      </c>
+      <c r="J44" s="9">
+        <v>0.93193342151675496</v>
+      </c>
+      <c r="K44" s="9">
+        <v>0.94006283068783103</v>
+      </c>
+      <c r="L44" s="9">
+        <v>0.84110449735449699</v>
+      </c>
+      <c r="M44" s="9">
+        <v>0.90436691651969403</v>
+      </c>
+      <c r="N44" s="9">
+        <v>4.4856230205271803E-2</v>
+      </c>
+      <c r="O44" s="9">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A45" s="8">
+        <v>5</v>
+      </c>
+      <c r="B45" s="9">
+        <v>24.257464090983099</v>
+      </c>
+      <c r="C45" s="9">
+        <v>8.1698787386534004</v>
+      </c>
+      <c r="D45" s="9">
+        <v>0.17366623878479001</v>
+      </c>
+      <c r="E45" s="9">
+        <v>1.2992691289136599E-3</v>
+      </c>
+      <c r="F45" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G45" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H45" s="9">
+        <v>0.03</v>
+      </c>
+      <c r="I45" s="9" t="s">
+        <v>517</v>
+      </c>
+      <c r="J45" s="9">
+        <v>0.86910273368606705</v>
+      </c>
+      <c r="K45" s="9">
+        <v>0.81564153439153397</v>
+      </c>
+      <c r="L45" s="9">
+        <v>0.98302469135802495</v>
+      </c>
+      <c r="M45" s="9">
+        <v>0.88925631981187503</v>
+      </c>
+      <c r="N45" s="9">
+        <v>6.9804038012686906E-2</v>
+      </c>
+      <c r="O45" s="9">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A46" s="8">
+        <v>6</v>
+      </c>
+      <c r="B46" s="9">
+        <v>16.5574656327566</v>
+      </c>
+      <c r="C46" s="9">
+        <v>1.35345099597561</v>
+      </c>
+      <c r="D46" s="9">
+        <v>0.19069115320841501</v>
+      </c>
+      <c r="E46" s="9">
+        <v>2.25673400768364E-3</v>
+      </c>
+      <c r="F46" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G46" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H46" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I46" s="9" t="s">
+        <v>518</v>
+      </c>
+      <c r="J46" s="9">
+        <v>0.71257716049382702</v>
+      </c>
+      <c r="K46" s="9">
+        <v>0.74710648148148195</v>
+      </c>
+      <c r="L46" s="9">
+        <v>0.731316137566138</v>
+      </c>
+      <c r="M46" s="9">
+        <v>0.73033325984714903</v>
+      </c>
+      <c r="N46" s="9">
+        <v>1.4113658595487801E-2</v>
+      </c>
+      <c r="O46" s="9">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A47" s="8">
+        <v>14</v>
+      </c>
+      <c r="B47" s="9">
+        <v>20.046814282735198</v>
+      </c>
+      <c r="C47" s="9">
+        <v>3.65246763128637</v>
+      </c>
+      <c r="D47" s="9">
+        <v>0.21114190419515</v>
+      </c>
+      <c r="E47" s="9">
+        <v>2.4935150604917002E-2</v>
+      </c>
+      <c r="F47" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G47" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H47" s="9">
+        <v>0.04</v>
+      </c>
+      <c r="I47" s="9" t="s">
+        <v>528</v>
+      </c>
+      <c r="J47" s="9">
+        <v>0.66093474426807797</v>
+      </c>
+      <c r="K47" s="9">
+        <v>0.76937279541446202</v>
+      </c>
+      <c r="L47" s="9">
+        <v>0.73506393298060002</v>
+      </c>
+      <c r="M47" s="9">
+        <v>0.72179049088771297</v>
+      </c>
+      <c r="N47" s="9">
+        <v>4.5253662340569302E-2</v>
+      </c>
+      <c r="O47" s="9">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A48" s="8">
+        <v>15</v>
+      </c>
+      <c r="B48" s="9">
+        <v>22.129306952158601</v>
+      </c>
+      <c r="C48" s="9">
+        <v>7.2613432135682698</v>
+      </c>
+      <c r="D48" s="9">
+        <v>0.202075004577637</v>
+      </c>
+      <c r="E48" s="9">
+        <v>1.36104236252903E-2</v>
+      </c>
+      <c r="F48" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G48" s="9" t="s">
+        <v>525</v>
+      </c>
+      <c r="H48" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I48" s="9" t="s">
+        <v>529</v>
+      </c>
+      <c r="J48" s="9">
+        <v>0.50002755731922399</v>
+      </c>
+      <c r="K48" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L48" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M48" s="9">
+        <v>0.50000918577307496</v>
+      </c>
+      <c r="N48" s="10">
+        <v>1.29906448630714E-5</v>
+      </c>
+      <c r="O48" s="9">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A49" s="8">
+        <v>7</v>
+      </c>
+      <c r="B49" s="9">
+        <v>51.968566417694099</v>
+      </c>
+      <c r="C49" s="9">
+        <v>19.183369264284998</v>
+      </c>
+      <c r="D49" s="9">
+        <v>0.241655031840007</v>
+      </c>
+      <c r="E49" s="9">
+        <v>5.57596348477448E-2</v>
+      </c>
+      <c r="F49" s="9">
+        <v>1E-4</v>
+      </c>
+      <c r="G49" s="9" t="s">
+        <v>515</v>
+      </c>
+      <c r="H49" s="9">
+        <v>0.1</v>
+      </c>
+      <c r="I49" s="9" t="s">
+        <v>519</v>
+      </c>
+      <c r="J49" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="K49" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="L49" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="M49" s="9">
+        <v>0.5</v>
+      </c>
+      <c r="N49" s="9">
+        <v>0</v>
+      </c>
+      <c r="O49" s="9">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="A1:O1" xr:uid="{C8D893D9-1BAA-9C49-916A-C91DC687D0E7}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:O49">
+      <sortCondition ref="O1:O49"/>
+    </sortState>
+  </autoFilter>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{25E002B6-4C3F-544B-BB8D-EEC765A7BC77}">
   <dimension ref="A1:S76"/>
   <sheetViews>
@@ -13433,12 +15984,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{966BA160-2365-7947-BA66-DCDE4697F731}">
   <dimension ref="A1:T73"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="T20" sqref="T20"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="X28" sqref="X28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17159,10 +19710,11 @@
     </sortState>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D0AC856-9B4F-924B-B602-6974E3ECE5F8}">
   <dimension ref="A1:T51"/>
   <sheetViews>

</xml_diff>